<commit_message>
Sync Github to OneDrive at 2024-ago
</commit_message>
<xml_diff>
--- a/documents/insumos/mapa_ods_ipea.xlsx
+++ b/documents/insumos/mapa_ods_ipea.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_080301F0B917EA879A95D4A0F882350324614ADF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71892CAA-80BE-43C4-B7B4-1E0EC67BB07F}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="11_080301F0B917EA879A95D4A0F882350324614ADF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5155DF1-AEA8-4060-9995-1403BF91D0E2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="11" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos" sheetId="1" r:id="rId1"/>
@@ -4886,7 +4886,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4902,6 +4902,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5001,12 +5007,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5043,6 +5043,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5090,9 +5099,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -5328,11 +5334,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="99.5703125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="25" customWidth="1"/>
-    <col min="5" max="16384" width="12.5703125" style="25"/>
+    <col min="1" max="1" width="4.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="99.5703125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="23" customWidth="1"/>
+    <col min="5" max="16384" width="12.5703125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="11.25">
@@ -5359,7 +5365,7 @@
       <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5373,7 +5379,7 @@
       <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5387,7 +5393,7 @@
       <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5401,7 +5407,7 @@
       <c r="C5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5415,7 +5421,7 @@
       <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="24" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5429,7 +5435,7 @@
       <c r="C7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5443,7 +5449,7 @@
       <c r="C8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5457,7 +5463,7 @@
       <c r="C9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5471,7 +5477,7 @@
       <c r="C10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="24" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5485,7 +5491,7 @@
       <c r="C11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="24" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5499,7 +5505,7 @@
       <c r="C12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="24" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5513,7 +5519,7 @@
       <c r="C13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5527,7 +5533,7 @@
       <c r="C14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="24" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5541,7 +5547,7 @@
       <c r="C15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5555,7 +5561,7 @@
       <c r="C16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="24" t="s">
         <v>63</v>
       </c>
     </row>
@@ -5569,21 +5575,21 @@
       <c r="C17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="24" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="11.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="24" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5618,16 +5624,17 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="B13:G16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="4" width="50.140625" customWidth="1"/>
+    <col min="6" max="6" width="63.5703125" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="12.75">
       <c r="A1" s="4" t="s">
         <v>76</v>
       </c>
@@ -5643,11 +5650,11 @@
       <c r="E1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="54.75">
       <c r="A2" s="16" t="s">
         <v>504</v>
       </c>
@@ -5657,17 +5664,17 @@
       <c r="C2" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>507</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="68.25">
       <c r="A3" s="16" t="s">
         <v>510</v>
       </c>
@@ -5683,7 +5690,7 @@
       <c r="E3" s="17" t="s">
         <v>514</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>515</v>
       </c>
     </row>
@@ -5703,18 +5710,18 @@
       <c r="E4" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:6" ht="27.75">
+      <c r="A5" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>523</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="42" t="s">
         <v>524</v>
       </c>
       <c r="D5" s="54" t="s">
@@ -5723,7 +5730,7 @@
       <c r="E5" s="17" t="s">
         <v>526</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>527</v>
       </c>
     </row>
@@ -5735,18 +5742,18 @@
       <c r="E6" s="16" t="s">
         <v>528</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:6" ht="27.75">
+      <c r="A7" s="42" t="s">
         <v>530</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="42" t="s">
         <v>532</v>
       </c>
       <c r="D7" s="56" t="s">
@@ -5755,7 +5762,7 @@
       <c r="E7" s="17" t="s">
         <v>534</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>535</v>
       </c>
     </row>
@@ -5767,7 +5774,7 @@
       <c r="E8" s="16" t="s">
         <v>536</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="16" t="s">
         <v>537</v>
       </c>
     </row>
@@ -5787,11 +5794,11 @@
       <c r="E9" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="83.25">
       <c r="A10" s="16" t="s">
         <v>544</v>
       </c>
@@ -5807,18 +5814,18 @@
       <c r="E10" s="17" t="s">
         <v>548</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="41" t="s">
+    <row r="11" spans="1:6" ht="27.75">
+      <c r="A11" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>551</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="42" t="s">
         <v>552</v>
       </c>
       <c r="D11" s="56" t="s">
@@ -5827,7 +5834,7 @@
       <c r="E11" s="17" t="s">
         <v>554</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>555</v>
       </c>
     </row>
@@ -5839,18 +5846,18 @@
       <c r="E12" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="16" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:6" ht="13.5">
+      <c r="A13" s="42" t="s">
         <v>558</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="42" t="s">
         <v>559</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="42" t="s">
         <v>560</v>
       </c>
       <c r="D13" s="56" t="s">
@@ -5859,7 +5866,7 @@
       <c r="E13" s="17" t="s">
         <v>562</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>563</v>
       </c>
     </row>
@@ -5871,18 +5878,18 @@
       <c r="E14" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="16" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>566</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="42" t="s">
         <v>567</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="42" t="s">
         <v>568</v>
       </c>
       <c r="D15" s="56" t="s">
@@ -5891,7 +5898,7 @@
       <c r="E15" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>571</v>
       </c>
     </row>
@@ -5903,7 +5910,7 @@
       <c r="E16" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="16" t="s">
         <v>573</v>
       </c>
     </row>
@@ -5920,11 +5927,11 @@
       <c r="E17" s="17" t="s">
         <v>577</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="17" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="83.25">
       <c r="A18" s="16" t="s">
         <v>579</v>
       </c>
@@ -5940,7 +5947,7 @@
       <c r="E18" s="17" t="s">
         <v>583</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="17" t="s">
         <v>584</v>
       </c>
     </row>
@@ -6010,16 +6017,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>585</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>586</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>587</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>588</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -6042,16 +6049,16 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>593</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>594</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="43" t="s">
         <v>595</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="41" t="s">
         <v>596</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -6074,16 +6081,16 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>601</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>602</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>603</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>604</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -6126,16 +6133,16 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>615</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>616</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="43" t="s">
         <v>617</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="40" t="s">
         <v>618</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -7261,7 +7268,7 @@
       <c r="E2" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="34" t="s">
         <v>645</v>
       </c>
     </row>
@@ -7281,7 +7288,7 @@
       <c r="E3" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="34" t="s">
         <v>651</v>
       </c>
     </row>
@@ -7321,7 +7328,7 @@
       <c r="E5" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="34" t="s">
         <v>662</v>
       </c>
     </row>
@@ -7366,13 +7373,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="40" t="s">
         <v>673</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>674</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="43" t="s">
         <v>675</v>
       </c>
       <c r="D8" s="56" t="s">
@@ -7388,7 +7395,7 @@
     <row r="9" spans="1:6" ht="12.75">
       <c r="A9" s="52"/>
       <c r="B9" s="52"/>
-      <c r="C9" s="43"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="52"/>
       <c r="E9" s="1" t="s">
         <v>679</v>
@@ -7545,13 +7552,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="69.75" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>709</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>710</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="43" t="s">
         <v>711</v>
       </c>
       <c r="D4" s="56" t="s">
@@ -7597,13 +7604,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="52.5" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>723</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>724</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="43" t="s">
         <v>725</v>
       </c>
       <c r="D7" s="56" t="s">
@@ -7629,13 +7636,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>730</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>731</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="43" t="s">
         <v>732</v>
       </c>
       <c r="D9" s="56" t="s">
@@ -7661,13 +7668,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="40" t="s">
         <v>738</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="43" t="s">
         <v>739</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>740</v>
       </c>
       <c r="D11" s="56" t="s">
@@ -7713,13 +7720,13 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="83.25" customHeight="1">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="40" t="s">
         <v>752</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="43" t="s">
         <v>753</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="43" t="s">
         <v>754</v>
       </c>
       <c r="D14" s="56" t="s">
@@ -7826,42 +7833,42 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>766</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>767</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>768</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>769</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>770</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>772</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>773</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>773</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>774</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="19" t="s">
         <v>775</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>776</v>
       </c>
     </row>
@@ -7870,50 +7877,50 @@
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
       <c r="D4" s="52"/>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>777</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>779</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>780</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>781</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>782</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>783</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="21" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>785</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="45" t="s">
         <v>786</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="45" t="s">
         <v>786</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>787</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>788</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="20" t="s">
         <v>789</v>
       </c>
     </row>
@@ -7922,150 +7929,150 @@
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
       <c r="D7" s="52"/>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>790</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="18" t="s">
         <v>792</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>793</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>794</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>795</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="20" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>798</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>799</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>800</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="26" t="s">
         <v>801</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>802</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="20" t="s">
         <v>803</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>804</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>805</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>806</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>807</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="19" t="s">
         <v>808</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="20" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="18" t="s">
         <v>810</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>811</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>812</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>813</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>814</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="20" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="18" t="s">
         <v>816</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>817</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>818</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>819</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="20" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="18" t="s">
         <v>821</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>822</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>823</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>824</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>825</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="20" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
         <v>827</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="18" t="s">
         <v>828</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>828</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>829</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="19" t="s">
         <v>830</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="20" t="s">
         <v>831</v>
       </c>
     </row>
@@ -9096,13 +9103,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>832</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>833</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>834</v>
       </c>
       <c r="D2" s="56" t="s">
@@ -9160,13 +9167,13 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>847</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="40" t="s">
         <v>848</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="40" t="s">
         <v>849</v>
       </c>
       <c r="D6" s="52"/>
@@ -10403,7 +10410,7 @@
       <c r="C9" s="1" t="s">
         <v>905</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="25" t="s">
         <v>906</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -10423,7 +10430,7 @@
       <c r="C10" s="1" t="s">
         <v>910</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="25" t="s">
         <v>911</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -11432,13 +11439,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="32"/>
-    <col min="2" max="2" width="50.140625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="85.42578125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="32"/>
-    <col min="6" max="6" width="60.7109375" style="32" customWidth="1"/>
-    <col min="7" max="16384" width="12.5703125" style="32"/>
+    <col min="1" max="1" width="12.5703125" style="30"/>
+    <col min="2" max="2" width="50.140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="30"/>
+    <col min="6" max="6" width="60.7109375" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="12.5703125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75">
@@ -11462,16 +11469,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>914</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>915</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>916</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>917</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -11482,14 +11489,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="33" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="31" t="s">
         <v>920</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="32" t="s">
         <v>921</v>
       </c>
     </row>
@@ -11509,7 +11516,7 @@
       <c r="E4" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="32" t="s">
         <v>927</v>
       </c>
     </row>
@@ -11529,39 +11536,39 @@
       <c r="E5" s="11" t="s">
         <v>931</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="32" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>933</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>934</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>934</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>935</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>936</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>937</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="11" t="s">
         <v>938</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="32" t="s">
         <v>939</v>
       </c>
     </row>
@@ -11581,7 +11588,7 @@
       <c r="E8" s="11" t="s">
         <v>944</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="32" t="s">
         <v>945</v>
       </c>
     </row>
@@ -11601,7 +11608,7 @@
       <c r="E9" s="11" t="s">
         <v>950</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="32" t="s">
         <v>951</v>
       </c>
     </row>
@@ -11621,7 +11628,7 @@
       <c r="E10" s="11" t="s">
         <v>956</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="32" t="s">
         <v>957</v>
       </c>
     </row>
@@ -11641,7 +11648,7 @@
       <c r="E11" s="11" t="s">
         <v>961</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="32" t="s">
         <v>962</v>
       </c>
     </row>
@@ -11661,7 +11668,7 @@
       <c r="E12" s="11" t="s">
         <v>967</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="32" t="s">
         <v>968</v>
       </c>
     </row>
@@ -11681,7 +11688,7 @@
       <c r="E13" s="11" t="s">
         <v>973</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="32" t="s">
         <v>974</v>
       </c>
     </row>
@@ -11701,7 +11708,7 @@
       <c r="E14" s="11" t="s">
         <v>979</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="32" t="s">
         <v>974</v>
       </c>
     </row>
@@ -11721,982 +11728,982 @@
       <c r="E15" s="11" t="s">
         <v>984</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="32" t="s">
         <v>957</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75"/>
-    <row r="17" s="32" customFormat="1" ht="12.75"/>
-    <row r="18" s="32" customFormat="1" ht="12.75"/>
-    <row r="19" s="32" customFormat="1" ht="12.75"/>
-    <row r="20" s="32" customFormat="1" ht="12.75"/>
-    <row r="21" s="32" customFormat="1" ht="12.75"/>
-    <row r="22" s="32" customFormat="1" ht="12.75"/>
-    <row r="23" s="32" customFormat="1" ht="12.75"/>
-    <row r="24" s="32" customFormat="1" ht="12.75"/>
-    <row r="25" s="32" customFormat="1" ht="12.75"/>
-    <row r="26" s="32" customFormat="1" ht="12.75"/>
-    <row r="27" s="32" customFormat="1" ht="12.75"/>
-    <row r="28" s="32" customFormat="1" ht="12.75"/>
-    <row r="29" s="32" customFormat="1" ht="12.75"/>
-    <row r="30" s="32" customFormat="1" ht="12.75"/>
-    <row r="31" s="32" customFormat="1" ht="12.75"/>
-    <row r="32" s="32" customFormat="1" ht="12.75"/>
-    <row r="33" s="32" customFormat="1" ht="12.75"/>
-    <row r="34" s="32" customFormat="1" ht="12.75"/>
-    <row r="35" s="32" customFormat="1" ht="12.75"/>
-    <row r="36" s="32" customFormat="1" ht="12.75"/>
-    <row r="37" s="32" customFormat="1" ht="12.75"/>
-    <row r="38" s="32" customFormat="1" ht="12.75"/>
-    <row r="39" s="32" customFormat="1" ht="12.75"/>
-    <row r="40" s="32" customFormat="1" ht="12.75"/>
-    <row r="41" s="32" customFormat="1" ht="12.75"/>
-    <row r="42" s="32" customFormat="1" ht="12.75"/>
-    <row r="43" s="32" customFormat="1" ht="12.75"/>
-    <row r="44" s="32" customFormat="1" ht="12.75"/>
-    <row r="45" s="32" customFormat="1" ht="12.75"/>
-    <row r="46" s="32" customFormat="1" ht="12.75"/>
-    <row r="47" s="32" customFormat="1" ht="12.75"/>
-    <row r="48" s="32" customFormat="1" ht="12.75"/>
-    <row r="49" s="32" customFormat="1" ht="12.75"/>
-    <row r="50" s="32" customFormat="1" ht="12.75"/>
-    <row r="51" s="32" customFormat="1" ht="12.75"/>
-    <row r="52" s="32" customFormat="1" ht="12.75"/>
-    <row r="53" s="32" customFormat="1" ht="12.75"/>
-    <row r="54" s="32" customFormat="1" ht="12.75"/>
-    <row r="55" s="32" customFormat="1" ht="12.75"/>
-    <row r="56" s="32" customFormat="1" ht="12.75"/>
-    <row r="57" s="32" customFormat="1" ht="12.75"/>
-    <row r="58" s="32" customFormat="1" ht="12.75"/>
-    <row r="59" s="32" customFormat="1" ht="12.75"/>
-    <row r="60" s="32" customFormat="1" ht="12.75"/>
-    <row r="61" s="32" customFormat="1" ht="12.75"/>
-    <row r="62" s="32" customFormat="1" ht="12.75"/>
-    <row r="63" s="32" customFormat="1" ht="12.75"/>
-    <row r="64" s="32" customFormat="1" ht="12.75"/>
-    <row r="65" s="32" customFormat="1" ht="12.75"/>
-    <row r="66" s="32" customFormat="1" ht="12.75"/>
-    <row r="67" s="32" customFormat="1" ht="12.75"/>
-    <row r="68" s="32" customFormat="1" ht="12.75"/>
-    <row r="69" s="32" customFormat="1" ht="12.75"/>
-    <row r="70" s="32" customFormat="1" ht="12.75"/>
-    <row r="71" s="32" customFormat="1" ht="12.75"/>
-    <row r="72" s="32" customFormat="1" ht="12.75"/>
-    <row r="73" s="32" customFormat="1" ht="12.75"/>
-    <row r="74" s="32" customFormat="1" ht="12.75"/>
-    <row r="75" s="32" customFormat="1" ht="12.75"/>
-    <row r="76" s="32" customFormat="1" ht="12.75"/>
-    <row r="77" s="32" customFormat="1" ht="12.75"/>
-    <row r="78" s="32" customFormat="1" ht="12.75"/>
-    <row r="79" s="32" customFormat="1" ht="12.75"/>
-    <row r="80" s="32" customFormat="1" ht="12.75"/>
-    <row r="81" s="32" customFormat="1" ht="12.75"/>
-    <row r="82" s="32" customFormat="1" ht="12.75"/>
-    <row r="83" s="32" customFormat="1" ht="12.75"/>
-    <row r="84" s="32" customFormat="1" ht="12.75"/>
-    <row r="85" s="32" customFormat="1" ht="12.75"/>
-    <row r="86" s="32" customFormat="1" ht="12.75"/>
-    <row r="87" s="32" customFormat="1" ht="12.75"/>
-    <row r="88" s="32" customFormat="1" ht="12.75"/>
-    <row r="89" s="32" customFormat="1" ht="12.75"/>
-    <row r="90" s="32" customFormat="1" ht="12.75"/>
-    <row r="91" s="32" customFormat="1" ht="12.75"/>
-    <row r="92" s="32" customFormat="1" ht="12.75"/>
-    <row r="93" s="32" customFormat="1" ht="12.75"/>
-    <row r="94" s="32" customFormat="1" ht="12.75"/>
-    <row r="95" s="32" customFormat="1" ht="12.75"/>
-    <row r="96" s="32" customFormat="1" ht="12.75"/>
-    <row r="97" s="32" customFormat="1" ht="12.75"/>
-    <row r="98" s="32" customFormat="1" ht="12.75"/>
-    <row r="99" s="32" customFormat="1" ht="12.75"/>
-    <row r="100" s="32" customFormat="1" ht="12.75"/>
-    <row r="101" s="32" customFormat="1" ht="12.75"/>
-    <row r="102" s="32" customFormat="1" ht="12.75"/>
-    <row r="103" s="32" customFormat="1" ht="12.75"/>
-    <row r="104" s="32" customFormat="1" ht="12.75"/>
-    <row r="105" s="32" customFormat="1" ht="12.75"/>
-    <row r="106" s="32" customFormat="1" ht="12.75"/>
-    <row r="107" s="32" customFormat="1" ht="12.75"/>
-    <row r="108" s="32" customFormat="1" ht="12.75"/>
-    <row r="109" s="32" customFormat="1" ht="12.75"/>
-    <row r="110" s="32" customFormat="1" ht="12.75"/>
-    <row r="111" s="32" customFormat="1" ht="12.75"/>
-    <row r="112" s="32" customFormat="1" ht="12.75"/>
-    <row r="113" s="32" customFormat="1" ht="12.75"/>
-    <row r="114" s="32" customFormat="1" ht="12.75"/>
-    <row r="115" s="32" customFormat="1" ht="12.75"/>
-    <row r="116" s="32" customFormat="1" ht="12.75"/>
-    <row r="117" s="32" customFormat="1" ht="12.75"/>
-    <row r="118" s="32" customFormat="1" ht="12.75"/>
-    <row r="119" s="32" customFormat="1" ht="12.75"/>
-    <row r="120" s="32" customFormat="1" ht="12.75"/>
-    <row r="121" s="32" customFormat="1" ht="12.75"/>
-    <row r="122" s="32" customFormat="1" ht="12.75"/>
-    <row r="123" s="32" customFormat="1" ht="12.75"/>
-    <row r="124" s="32" customFormat="1" ht="12.75"/>
-    <row r="125" s="32" customFormat="1" ht="12.75"/>
-    <row r="126" s="32" customFormat="1" ht="12.75"/>
-    <row r="127" s="32" customFormat="1" ht="12.75"/>
-    <row r="128" s="32" customFormat="1" ht="12.75"/>
-    <row r="129" s="32" customFormat="1" ht="12.75"/>
-    <row r="130" s="32" customFormat="1" ht="12.75"/>
-    <row r="131" s="32" customFormat="1" ht="12.75"/>
-    <row r="132" s="32" customFormat="1" ht="12.75"/>
-    <row r="133" s="32" customFormat="1" ht="12.75"/>
-    <row r="134" s="32" customFormat="1" ht="12.75"/>
-    <row r="135" s="32" customFormat="1" ht="12.75"/>
-    <row r="136" s="32" customFormat="1" ht="12.75"/>
-    <row r="137" s="32" customFormat="1" ht="12.75"/>
-    <row r="138" s="32" customFormat="1" ht="12.75"/>
-    <row r="139" s="32" customFormat="1" ht="12.75"/>
-    <row r="140" s="32" customFormat="1" ht="12.75"/>
-    <row r="141" s="32" customFormat="1" ht="12.75"/>
-    <row r="142" s="32" customFormat="1" ht="12.75"/>
-    <row r="143" s="32" customFormat="1" ht="12.75"/>
-    <row r="144" s="32" customFormat="1" ht="12.75"/>
-    <row r="145" s="32" customFormat="1" ht="12.75"/>
-    <row r="146" s="32" customFormat="1" ht="12.75"/>
-    <row r="147" s="32" customFormat="1" ht="12.75"/>
-    <row r="148" s="32" customFormat="1" ht="12.75"/>
-    <row r="149" s="32" customFormat="1" ht="12.75"/>
-    <row r="150" s="32" customFormat="1" ht="12.75"/>
-    <row r="151" s="32" customFormat="1" ht="12.75"/>
-    <row r="152" s="32" customFormat="1" ht="12.75"/>
-    <row r="153" s="32" customFormat="1" ht="12.75"/>
-    <row r="154" s="32" customFormat="1" ht="12.75"/>
-    <row r="155" s="32" customFormat="1" ht="12.75"/>
-    <row r="156" s="32" customFormat="1" ht="12.75"/>
-    <row r="157" s="32" customFormat="1" ht="12.75"/>
-    <row r="158" s="32" customFormat="1" ht="12.75"/>
-    <row r="159" s="32" customFormat="1" ht="12.75"/>
-    <row r="160" s="32" customFormat="1" ht="12.75"/>
-    <row r="161" s="32" customFormat="1" ht="12.75"/>
-    <row r="162" s="32" customFormat="1" ht="12.75"/>
-    <row r="163" s="32" customFormat="1" ht="12.75"/>
-    <row r="164" s="32" customFormat="1" ht="12.75"/>
-    <row r="165" s="32" customFormat="1" ht="12.75"/>
-    <row r="166" s="32" customFormat="1" ht="12.75"/>
-    <row r="167" s="32" customFormat="1" ht="12.75"/>
-    <row r="168" s="32" customFormat="1" ht="12.75"/>
-    <row r="169" s="32" customFormat="1" ht="12.75"/>
-    <row r="170" s="32" customFormat="1" ht="12.75"/>
-    <row r="171" s="32" customFormat="1" ht="12.75"/>
-    <row r="172" s="32" customFormat="1" ht="12.75"/>
-    <row r="173" s="32" customFormat="1" ht="12.75"/>
-    <row r="174" s="32" customFormat="1" ht="12.75"/>
-    <row r="175" s="32" customFormat="1" ht="12.75"/>
-    <row r="176" s="32" customFormat="1" ht="12.75"/>
-    <row r="177" s="32" customFormat="1" ht="12.75"/>
-    <row r="178" s="32" customFormat="1" ht="12.75"/>
-    <row r="179" s="32" customFormat="1" ht="12.75"/>
-    <row r="180" s="32" customFormat="1" ht="12.75"/>
-    <row r="181" s="32" customFormat="1" ht="12.75"/>
-    <row r="182" s="32" customFormat="1" ht="12.75"/>
-    <row r="183" s="32" customFormat="1" ht="12.75"/>
-    <row r="184" s="32" customFormat="1" ht="12.75"/>
-    <row r="185" s="32" customFormat="1" ht="12.75"/>
-    <row r="186" s="32" customFormat="1" ht="12.75"/>
-    <row r="187" s="32" customFormat="1" ht="12.75"/>
-    <row r="188" s="32" customFormat="1" ht="12.75"/>
-    <row r="189" s="32" customFormat="1" ht="12.75"/>
-    <row r="190" s="32" customFormat="1" ht="12.75"/>
-    <row r="191" s="32" customFormat="1" ht="12.75"/>
-    <row r="192" s="32" customFormat="1" ht="12.75"/>
-    <row r="193" s="32" customFormat="1" ht="12.75"/>
-    <row r="194" s="32" customFormat="1" ht="12.75"/>
-    <row r="195" s="32" customFormat="1" ht="12.75"/>
-    <row r="196" s="32" customFormat="1" ht="12.75"/>
-    <row r="197" s="32" customFormat="1" ht="12.75"/>
-    <row r="198" s="32" customFormat="1" ht="12.75"/>
-    <row r="199" s="32" customFormat="1" ht="12.75"/>
-    <row r="200" s="32" customFormat="1" ht="12.75"/>
-    <row r="201" s="32" customFormat="1" ht="12.75"/>
-    <row r="202" s="32" customFormat="1" ht="12.75"/>
-    <row r="203" s="32" customFormat="1" ht="12.75"/>
-    <row r="204" s="32" customFormat="1" ht="12.75"/>
-    <row r="205" s="32" customFormat="1" ht="12.75"/>
-    <row r="206" s="32" customFormat="1" ht="12.75"/>
-    <row r="207" s="32" customFormat="1" ht="12.75"/>
-    <row r="208" s="32" customFormat="1" ht="12.75"/>
-    <row r="209" s="32" customFormat="1" ht="12.75"/>
-    <row r="210" s="32" customFormat="1" ht="12.75"/>
-    <row r="211" s="32" customFormat="1" ht="12.75"/>
-    <row r="212" s="32" customFormat="1" ht="12.75"/>
-    <row r="213" s="32" customFormat="1" ht="12.75"/>
-    <row r="214" s="32" customFormat="1" ht="12.75"/>
-    <row r="215" s="32" customFormat="1" ht="12.75"/>
-    <row r="216" s="32" customFormat="1" ht="12.75"/>
-    <row r="217" s="32" customFormat="1" ht="12.75"/>
-    <row r="218" s="32" customFormat="1" ht="12.75"/>
-    <row r="219" s="32" customFormat="1" ht="12.75"/>
-    <row r="220" s="32" customFormat="1" ht="12.75"/>
-    <row r="221" s="32" customFormat="1" ht="12.75"/>
-    <row r="222" s="32" customFormat="1" ht="12.75"/>
-    <row r="223" s="32" customFormat="1" ht="12.75"/>
-    <row r="224" s="32" customFormat="1" ht="12.75"/>
-    <row r="225" s="32" customFormat="1" ht="12.75"/>
-    <row r="226" s="32" customFormat="1" ht="12.75"/>
-    <row r="227" s="32" customFormat="1" ht="12.75"/>
-    <row r="228" s="32" customFormat="1" ht="12.75"/>
-    <row r="229" s="32" customFormat="1" ht="12.75"/>
-    <row r="230" s="32" customFormat="1" ht="12.75"/>
-    <row r="231" s="32" customFormat="1" ht="12.75"/>
-    <row r="232" s="32" customFormat="1" ht="12.75"/>
-    <row r="233" s="32" customFormat="1" ht="12.75"/>
-    <row r="234" s="32" customFormat="1" ht="12.75"/>
-    <row r="235" s="32" customFormat="1" ht="12.75"/>
-    <row r="236" s="32" customFormat="1" ht="12.75"/>
-    <row r="237" s="32" customFormat="1" ht="12.75"/>
-    <row r="238" s="32" customFormat="1" ht="12.75"/>
-    <row r="239" s="32" customFormat="1" ht="12.75"/>
-    <row r="240" s="32" customFormat="1" ht="12.75"/>
-    <row r="241" s="32" customFormat="1" ht="12.75"/>
-    <row r="242" s="32" customFormat="1" ht="12.75"/>
-    <row r="243" s="32" customFormat="1" ht="12.75"/>
-    <row r="244" s="32" customFormat="1" ht="12.75"/>
-    <row r="245" s="32" customFormat="1" ht="12.75"/>
-    <row r="246" s="32" customFormat="1" ht="12.75"/>
-    <row r="247" s="32" customFormat="1" ht="12.75"/>
-    <row r="248" s="32" customFormat="1" ht="12.75"/>
-    <row r="249" s="32" customFormat="1" ht="12.75"/>
-    <row r="250" s="32" customFormat="1" ht="12.75"/>
-    <row r="251" s="32" customFormat="1" ht="12.75"/>
-    <row r="252" s="32" customFormat="1" ht="12.75"/>
-    <row r="253" s="32" customFormat="1" ht="12.75"/>
-    <row r="254" s="32" customFormat="1" ht="12.75"/>
-    <row r="255" s="32" customFormat="1" ht="12.75"/>
-    <row r="256" s="32" customFormat="1" ht="12.75"/>
-    <row r="257" s="32" customFormat="1" ht="12.75"/>
-    <row r="258" s="32" customFormat="1" ht="12.75"/>
-    <row r="259" s="32" customFormat="1" ht="12.75"/>
-    <row r="260" s="32" customFormat="1" ht="12.75"/>
-    <row r="261" s="32" customFormat="1" ht="12.75"/>
-    <row r="262" s="32" customFormat="1" ht="12.75"/>
-    <row r="263" s="32" customFormat="1" ht="12.75"/>
-    <row r="264" s="32" customFormat="1" ht="12.75"/>
-    <row r="265" s="32" customFormat="1" ht="12.75"/>
-    <row r="266" s="32" customFormat="1" ht="12.75"/>
-    <row r="267" s="32" customFormat="1" ht="12.75"/>
-    <row r="268" s="32" customFormat="1" ht="12.75"/>
-    <row r="269" s="32" customFormat="1" ht="12.75"/>
-    <row r="270" s="32" customFormat="1" ht="12.75"/>
-    <row r="271" s="32" customFormat="1" ht="12.75"/>
-    <row r="272" s="32" customFormat="1" ht="12.75"/>
-    <row r="273" s="32" customFormat="1" ht="12.75"/>
-    <row r="274" s="32" customFormat="1" ht="12.75"/>
-    <row r="275" s="32" customFormat="1" ht="12.75"/>
-    <row r="276" s="32" customFormat="1" ht="12.75"/>
-    <row r="277" s="32" customFormat="1" ht="12.75"/>
-    <row r="278" s="32" customFormat="1" ht="12.75"/>
-    <row r="279" s="32" customFormat="1" ht="12.75"/>
-    <row r="280" s="32" customFormat="1" ht="12.75"/>
-    <row r="281" s="32" customFormat="1" ht="12.75"/>
-    <row r="282" s="32" customFormat="1" ht="12.75"/>
-    <row r="283" s="32" customFormat="1" ht="12.75"/>
-    <row r="284" s="32" customFormat="1" ht="12.75"/>
-    <row r="285" s="32" customFormat="1" ht="12.75"/>
-    <row r="286" s="32" customFormat="1" ht="12.75"/>
-    <row r="287" s="32" customFormat="1" ht="12.75"/>
-    <row r="288" s="32" customFormat="1" ht="12.75"/>
-    <row r="289" s="32" customFormat="1" ht="12.75"/>
-    <row r="290" s="32" customFormat="1" ht="12.75"/>
-    <row r="291" s="32" customFormat="1" ht="12.75"/>
-    <row r="292" s="32" customFormat="1" ht="12.75"/>
-    <row r="293" s="32" customFormat="1" ht="12.75"/>
-    <row r="294" s="32" customFormat="1" ht="12.75"/>
-    <row r="295" s="32" customFormat="1" ht="12.75"/>
-    <row r="296" s="32" customFormat="1" ht="12.75"/>
-    <row r="297" s="32" customFormat="1" ht="12.75"/>
-    <row r="298" s="32" customFormat="1" ht="12.75"/>
-    <row r="299" s="32" customFormat="1" ht="12.75"/>
-    <row r="300" s="32" customFormat="1" ht="12.75"/>
-    <row r="301" s="32" customFormat="1" ht="12.75"/>
-    <row r="302" s="32" customFormat="1" ht="12.75"/>
-    <row r="303" s="32" customFormat="1" ht="12.75"/>
-    <row r="304" s="32" customFormat="1" ht="12.75"/>
-    <row r="305" s="32" customFormat="1" ht="12.75"/>
-    <row r="306" s="32" customFormat="1" ht="12.75"/>
-    <row r="307" s="32" customFormat="1" ht="12.75"/>
-    <row r="308" s="32" customFormat="1" ht="12.75"/>
-    <row r="309" s="32" customFormat="1" ht="12.75"/>
-    <row r="310" s="32" customFormat="1" ht="12.75"/>
-    <row r="311" s="32" customFormat="1" ht="12.75"/>
-    <row r="312" s="32" customFormat="1" ht="12.75"/>
-    <row r="313" s="32" customFormat="1" ht="12.75"/>
-    <row r="314" s="32" customFormat="1" ht="12.75"/>
-    <row r="315" s="32" customFormat="1" ht="12.75"/>
-    <row r="316" s="32" customFormat="1" ht="12.75"/>
-    <row r="317" s="32" customFormat="1" ht="12.75"/>
-    <row r="318" s="32" customFormat="1" ht="12.75"/>
-    <row r="319" s="32" customFormat="1" ht="12.75"/>
-    <row r="320" s="32" customFormat="1" ht="12.75"/>
-    <row r="321" s="32" customFormat="1" ht="12.75"/>
-    <row r="322" s="32" customFormat="1" ht="12.75"/>
-    <row r="323" s="32" customFormat="1" ht="12.75"/>
-    <row r="324" s="32" customFormat="1" ht="12.75"/>
-    <row r="325" s="32" customFormat="1" ht="12.75"/>
-    <row r="326" s="32" customFormat="1" ht="12.75"/>
-    <row r="327" s="32" customFormat="1" ht="12.75"/>
-    <row r="328" s="32" customFormat="1" ht="12.75"/>
-    <row r="329" s="32" customFormat="1" ht="12.75"/>
-    <row r="330" s="32" customFormat="1" ht="12.75"/>
-    <row r="331" s="32" customFormat="1" ht="12.75"/>
-    <row r="332" s="32" customFormat="1" ht="12.75"/>
-    <row r="333" s="32" customFormat="1" ht="12.75"/>
-    <row r="334" s="32" customFormat="1" ht="12.75"/>
-    <row r="335" s="32" customFormat="1" ht="12.75"/>
-    <row r="336" s="32" customFormat="1" ht="12.75"/>
-    <row r="337" s="32" customFormat="1" ht="12.75"/>
-    <row r="338" s="32" customFormat="1" ht="12.75"/>
-    <row r="339" s="32" customFormat="1" ht="12.75"/>
-    <row r="340" s="32" customFormat="1" ht="12.75"/>
-    <row r="341" s="32" customFormat="1" ht="12.75"/>
-    <row r="342" s="32" customFormat="1" ht="12.75"/>
-    <row r="343" s="32" customFormat="1" ht="12.75"/>
-    <row r="344" s="32" customFormat="1" ht="12.75"/>
-    <row r="345" s="32" customFormat="1" ht="12.75"/>
-    <row r="346" s="32" customFormat="1" ht="12.75"/>
-    <row r="347" s="32" customFormat="1" ht="12.75"/>
-    <row r="348" s="32" customFormat="1" ht="12.75"/>
-    <row r="349" s="32" customFormat="1" ht="12.75"/>
-    <row r="350" s="32" customFormat="1" ht="12.75"/>
-    <row r="351" s="32" customFormat="1" ht="12.75"/>
-    <row r="352" s="32" customFormat="1" ht="12.75"/>
-    <row r="353" s="32" customFormat="1" ht="12.75"/>
-    <row r="354" s="32" customFormat="1" ht="12.75"/>
-    <row r="355" s="32" customFormat="1" ht="12.75"/>
-    <row r="356" s="32" customFormat="1" ht="12.75"/>
-    <row r="357" s="32" customFormat="1" ht="12.75"/>
-    <row r="358" s="32" customFormat="1" ht="12.75"/>
-    <row r="359" s="32" customFormat="1" ht="12.75"/>
-    <row r="360" s="32" customFormat="1" ht="12.75"/>
-    <row r="361" s="32" customFormat="1" ht="12.75"/>
-    <row r="362" s="32" customFormat="1" ht="12.75"/>
-    <row r="363" s="32" customFormat="1" ht="12.75"/>
-    <row r="364" s="32" customFormat="1" ht="12.75"/>
-    <row r="365" s="32" customFormat="1" ht="12.75"/>
-    <row r="366" s="32" customFormat="1" ht="12.75"/>
-    <row r="367" s="32" customFormat="1" ht="12.75"/>
-    <row r="368" s="32" customFormat="1" ht="12.75"/>
-    <row r="369" s="32" customFormat="1" ht="12.75"/>
-    <row r="370" s="32" customFormat="1" ht="12.75"/>
-    <row r="371" s="32" customFormat="1" ht="12.75"/>
-    <row r="372" s="32" customFormat="1" ht="12.75"/>
-    <row r="373" s="32" customFormat="1" ht="12.75"/>
-    <row r="374" s="32" customFormat="1" ht="12.75"/>
-    <row r="375" s="32" customFormat="1" ht="12.75"/>
-    <row r="376" s="32" customFormat="1" ht="12.75"/>
-    <row r="377" s="32" customFormat="1" ht="12.75"/>
-    <row r="378" s="32" customFormat="1" ht="12.75"/>
-    <row r="379" s="32" customFormat="1" ht="12.75"/>
-    <row r="380" s="32" customFormat="1" ht="12.75"/>
-    <row r="381" s="32" customFormat="1" ht="12.75"/>
-    <row r="382" s="32" customFormat="1" ht="12.75"/>
-    <row r="383" s="32" customFormat="1" ht="12.75"/>
-    <row r="384" s="32" customFormat="1" ht="12.75"/>
-    <row r="385" s="32" customFormat="1" ht="12.75"/>
-    <row r="386" s="32" customFormat="1" ht="12.75"/>
-    <row r="387" s="32" customFormat="1" ht="12.75"/>
-    <row r="388" s="32" customFormat="1" ht="12.75"/>
-    <row r="389" s="32" customFormat="1" ht="12.75"/>
-    <row r="390" s="32" customFormat="1" ht="12.75"/>
-    <row r="391" s="32" customFormat="1" ht="12.75"/>
-    <row r="392" s="32" customFormat="1" ht="12.75"/>
-    <row r="393" s="32" customFormat="1" ht="12.75"/>
-    <row r="394" s="32" customFormat="1" ht="12.75"/>
-    <row r="395" s="32" customFormat="1" ht="12.75"/>
-    <row r="396" s="32" customFormat="1" ht="12.75"/>
-    <row r="397" s="32" customFormat="1" ht="12.75"/>
-    <row r="398" s="32" customFormat="1" ht="12.75"/>
-    <row r="399" s="32" customFormat="1" ht="12.75"/>
-    <row r="400" s="32" customFormat="1" ht="12.75"/>
-    <row r="401" s="32" customFormat="1" ht="12.75"/>
-    <row r="402" s="32" customFormat="1" ht="12.75"/>
-    <row r="403" s="32" customFormat="1" ht="12.75"/>
-    <row r="404" s="32" customFormat="1" ht="12.75"/>
-    <row r="405" s="32" customFormat="1" ht="12.75"/>
-    <row r="406" s="32" customFormat="1" ht="12.75"/>
-    <row r="407" s="32" customFormat="1" ht="12.75"/>
-    <row r="408" s="32" customFormat="1" ht="12.75"/>
-    <row r="409" s="32" customFormat="1" ht="12.75"/>
-    <row r="410" s="32" customFormat="1" ht="12.75"/>
-    <row r="411" s="32" customFormat="1" ht="12.75"/>
-    <row r="412" s="32" customFormat="1" ht="12.75"/>
-    <row r="413" s="32" customFormat="1" ht="12.75"/>
-    <row r="414" s="32" customFormat="1" ht="12.75"/>
-    <row r="415" s="32" customFormat="1" ht="12.75"/>
-    <row r="416" s="32" customFormat="1" ht="12.75"/>
-    <row r="417" s="32" customFormat="1" ht="12.75"/>
-    <row r="418" s="32" customFormat="1" ht="12.75"/>
-    <row r="419" s="32" customFormat="1" ht="12.75"/>
-    <row r="420" s="32" customFormat="1" ht="12.75"/>
-    <row r="421" s="32" customFormat="1" ht="12.75"/>
-    <row r="422" s="32" customFormat="1" ht="12.75"/>
-    <row r="423" s="32" customFormat="1" ht="12.75"/>
-    <row r="424" s="32" customFormat="1" ht="12.75"/>
-    <row r="425" s="32" customFormat="1" ht="12.75"/>
-    <row r="426" s="32" customFormat="1" ht="12.75"/>
-    <row r="427" s="32" customFormat="1" ht="12.75"/>
-    <row r="428" s="32" customFormat="1" ht="12.75"/>
-    <row r="429" s="32" customFormat="1" ht="12.75"/>
-    <row r="430" s="32" customFormat="1" ht="12.75"/>
-    <row r="431" s="32" customFormat="1" ht="12.75"/>
-    <row r="432" s="32" customFormat="1" ht="12.75"/>
-    <row r="433" s="32" customFormat="1" ht="12.75"/>
-    <row r="434" s="32" customFormat="1" ht="12.75"/>
-    <row r="435" s="32" customFormat="1" ht="12.75"/>
-    <row r="436" s="32" customFormat="1" ht="12.75"/>
-    <row r="437" s="32" customFormat="1" ht="12.75"/>
-    <row r="438" s="32" customFormat="1" ht="12.75"/>
-    <row r="439" s="32" customFormat="1" ht="12.75"/>
-    <row r="440" s="32" customFormat="1" ht="12.75"/>
-    <row r="441" s="32" customFormat="1" ht="12.75"/>
-    <row r="442" s="32" customFormat="1" ht="12.75"/>
-    <row r="443" s="32" customFormat="1" ht="12.75"/>
-    <row r="444" s="32" customFormat="1" ht="12.75"/>
-    <row r="445" s="32" customFormat="1" ht="12.75"/>
-    <row r="446" s="32" customFormat="1" ht="12.75"/>
-    <row r="447" s="32" customFormat="1" ht="12.75"/>
-    <row r="448" s="32" customFormat="1" ht="12.75"/>
-    <row r="449" s="32" customFormat="1" ht="12.75"/>
-    <row r="450" s="32" customFormat="1" ht="12.75"/>
-    <row r="451" s="32" customFormat="1" ht="12.75"/>
-    <row r="452" s="32" customFormat="1" ht="12.75"/>
-    <row r="453" s="32" customFormat="1" ht="12.75"/>
-    <row r="454" s="32" customFormat="1" ht="12.75"/>
-    <row r="455" s="32" customFormat="1" ht="12.75"/>
-    <row r="456" s="32" customFormat="1" ht="12.75"/>
-    <row r="457" s="32" customFormat="1" ht="12.75"/>
-    <row r="458" s="32" customFormat="1" ht="12.75"/>
-    <row r="459" s="32" customFormat="1" ht="12.75"/>
-    <row r="460" s="32" customFormat="1" ht="12.75"/>
-    <row r="461" s="32" customFormat="1" ht="12.75"/>
-    <row r="462" s="32" customFormat="1" ht="12.75"/>
-    <row r="463" s="32" customFormat="1" ht="12.75"/>
-    <row r="464" s="32" customFormat="1" ht="12.75"/>
-    <row r="465" s="32" customFormat="1" ht="12.75"/>
-    <row r="466" s="32" customFormat="1" ht="12.75"/>
-    <row r="467" s="32" customFormat="1" ht="12.75"/>
-    <row r="468" s="32" customFormat="1" ht="12.75"/>
-    <row r="469" s="32" customFormat="1" ht="12.75"/>
-    <row r="470" s="32" customFormat="1" ht="12.75"/>
-    <row r="471" s="32" customFormat="1" ht="12.75"/>
-    <row r="472" s="32" customFormat="1" ht="12.75"/>
-    <row r="473" s="32" customFormat="1" ht="12.75"/>
-    <row r="474" s="32" customFormat="1" ht="12.75"/>
-    <row r="475" s="32" customFormat="1" ht="12.75"/>
-    <row r="476" s="32" customFormat="1" ht="12.75"/>
-    <row r="477" s="32" customFormat="1" ht="12.75"/>
-    <row r="478" s="32" customFormat="1" ht="12.75"/>
-    <row r="479" s="32" customFormat="1" ht="12.75"/>
-    <row r="480" s="32" customFormat="1" ht="12.75"/>
-    <row r="481" s="32" customFormat="1" ht="12.75"/>
-    <row r="482" s="32" customFormat="1" ht="12.75"/>
-    <row r="483" s="32" customFormat="1" ht="12.75"/>
-    <row r="484" s="32" customFormat="1" ht="12.75"/>
-    <row r="485" s="32" customFormat="1" ht="12.75"/>
-    <row r="486" s="32" customFormat="1" ht="12.75"/>
-    <row r="487" s="32" customFormat="1" ht="12.75"/>
-    <row r="488" s="32" customFormat="1" ht="12.75"/>
-    <row r="489" s="32" customFormat="1" ht="12.75"/>
-    <row r="490" s="32" customFormat="1" ht="12.75"/>
-    <row r="491" s="32" customFormat="1" ht="12.75"/>
-    <row r="492" s="32" customFormat="1" ht="12.75"/>
-    <row r="493" s="32" customFormat="1" ht="12.75"/>
-    <row r="494" s="32" customFormat="1" ht="12.75"/>
-    <row r="495" s="32" customFormat="1" ht="12.75"/>
-    <row r="496" s="32" customFormat="1" ht="12.75"/>
-    <row r="497" s="32" customFormat="1" ht="12.75"/>
-    <row r="498" s="32" customFormat="1" ht="12.75"/>
-    <row r="499" s="32" customFormat="1" ht="12.75"/>
-    <row r="500" s="32" customFormat="1" ht="12.75"/>
-    <row r="501" s="32" customFormat="1" ht="12.75"/>
-    <row r="502" s="32" customFormat="1" ht="12.75"/>
-    <row r="503" s="32" customFormat="1" ht="12.75"/>
-    <row r="504" s="32" customFormat="1" ht="12.75"/>
-    <row r="505" s="32" customFormat="1" ht="12.75"/>
-    <row r="506" s="32" customFormat="1" ht="12.75"/>
-    <row r="507" s="32" customFormat="1" ht="12.75"/>
-    <row r="508" s="32" customFormat="1" ht="12.75"/>
-    <row r="509" s="32" customFormat="1" ht="12.75"/>
-    <row r="510" s="32" customFormat="1" ht="12.75"/>
-    <row r="511" s="32" customFormat="1" ht="12.75"/>
-    <row r="512" s="32" customFormat="1" ht="12.75"/>
-    <row r="513" s="32" customFormat="1" ht="12.75"/>
-    <row r="514" s="32" customFormat="1" ht="12.75"/>
-    <row r="515" s="32" customFormat="1" ht="12.75"/>
-    <row r="516" s="32" customFormat="1" ht="12.75"/>
-    <row r="517" s="32" customFormat="1" ht="12.75"/>
-    <row r="518" s="32" customFormat="1" ht="12.75"/>
-    <row r="519" s="32" customFormat="1" ht="12.75"/>
-    <row r="520" s="32" customFormat="1" ht="12.75"/>
-    <row r="521" s="32" customFormat="1" ht="12.75"/>
-    <row r="522" s="32" customFormat="1" ht="12.75"/>
-    <row r="523" s="32" customFormat="1" ht="12.75"/>
-    <row r="524" s="32" customFormat="1" ht="12.75"/>
-    <row r="525" s="32" customFormat="1" ht="12.75"/>
-    <row r="526" s="32" customFormat="1" ht="12.75"/>
-    <row r="527" s="32" customFormat="1" ht="12.75"/>
-    <row r="528" s="32" customFormat="1" ht="12.75"/>
-    <row r="529" s="32" customFormat="1" ht="12.75"/>
-    <row r="530" s="32" customFormat="1" ht="12.75"/>
-    <row r="531" s="32" customFormat="1" ht="12.75"/>
-    <row r="532" s="32" customFormat="1" ht="12.75"/>
-    <row r="533" s="32" customFormat="1" ht="12.75"/>
-    <row r="534" s="32" customFormat="1" ht="12.75"/>
-    <row r="535" s="32" customFormat="1" ht="12.75"/>
-    <row r="536" s="32" customFormat="1" ht="12.75"/>
-    <row r="537" s="32" customFormat="1" ht="12.75"/>
-    <row r="538" s="32" customFormat="1" ht="12.75"/>
-    <row r="539" s="32" customFormat="1" ht="12.75"/>
-    <row r="540" s="32" customFormat="1" ht="12.75"/>
-    <row r="541" s="32" customFormat="1" ht="12.75"/>
-    <row r="542" s="32" customFormat="1" ht="12.75"/>
-    <row r="543" s="32" customFormat="1" ht="12.75"/>
-    <row r="544" s="32" customFormat="1" ht="12.75"/>
-    <row r="545" s="32" customFormat="1" ht="12.75"/>
-    <row r="546" s="32" customFormat="1" ht="12.75"/>
-    <row r="547" s="32" customFormat="1" ht="12.75"/>
-    <row r="548" s="32" customFormat="1" ht="12.75"/>
-    <row r="549" s="32" customFormat="1" ht="12.75"/>
-    <row r="550" s="32" customFormat="1" ht="12.75"/>
-    <row r="551" s="32" customFormat="1" ht="12.75"/>
-    <row r="552" s="32" customFormat="1" ht="12.75"/>
-    <row r="553" s="32" customFormat="1" ht="12.75"/>
-    <row r="554" s="32" customFormat="1" ht="12.75"/>
-    <row r="555" s="32" customFormat="1" ht="12.75"/>
-    <row r="556" s="32" customFormat="1" ht="12.75"/>
-    <row r="557" s="32" customFormat="1" ht="12.75"/>
-    <row r="558" s="32" customFormat="1" ht="12.75"/>
-    <row r="559" s="32" customFormat="1" ht="12.75"/>
-    <row r="560" s="32" customFormat="1" ht="12.75"/>
-    <row r="561" s="32" customFormat="1" ht="12.75"/>
-    <row r="562" s="32" customFormat="1" ht="12.75"/>
-    <row r="563" s="32" customFormat="1" ht="12.75"/>
-    <row r="564" s="32" customFormat="1" ht="12.75"/>
-    <row r="565" s="32" customFormat="1" ht="12.75"/>
-    <row r="566" s="32" customFormat="1" ht="12.75"/>
-    <row r="567" s="32" customFormat="1" ht="12.75"/>
-    <row r="568" s="32" customFormat="1" ht="12.75"/>
-    <row r="569" s="32" customFormat="1" ht="12.75"/>
-    <row r="570" s="32" customFormat="1" ht="12.75"/>
-    <row r="571" s="32" customFormat="1" ht="12.75"/>
-    <row r="572" s="32" customFormat="1" ht="12.75"/>
-    <row r="573" s="32" customFormat="1" ht="12.75"/>
-    <row r="574" s="32" customFormat="1" ht="12.75"/>
-    <row r="575" s="32" customFormat="1" ht="12.75"/>
-    <row r="576" s="32" customFormat="1" ht="12.75"/>
-    <row r="577" s="32" customFormat="1" ht="12.75"/>
-    <row r="578" s="32" customFormat="1" ht="12.75"/>
-    <row r="579" s="32" customFormat="1" ht="12.75"/>
-    <row r="580" s="32" customFormat="1" ht="12.75"/>
-    <row r="581" s="32" customFormat="1" ht="12.75"/>
-    <row r="582" s="32" customFormat="1" ht="12.75"/>
-    <row r="583" s="32" customFormat="1" ht="12.75"/>
-    <row r="584" s="32" customFormat="1" ht="12.75"/>
-    <row r="585" s="32" customFormat="1" ht="12.75"/>
-    <row r="586" s="32" customFormat="1" ht="12.75"/>
-    <row r="587" s="32" customFormat="1" ht="12.75"/>
-    <row r="588" s="32" customFormat="1" ht="12.75"/>
-    <row r="589" s="32" customFormat="1" ht="12.75"/>
-    <row r="590" s="32" customFormat="1" ht="12.75"/>
-    <row r="591" s="32" customFormat="1" ht="12.75"/>
-    <row r="592" s="32" customFormat="1" ht="12.75"/>
-    <row r="593" s="32" customFormat="1" ht="12.75"/>
-    <row r="594" s="32" customFormat="1" ht="12.75"/>
-    <row r="595" s="32" customFormat="1" ht="12.75"/>
-    <row r="596" s="32" customFormat="1" ht="12.75"/>
-    <row r="597" s="32" customFormat="1" ht="12.75"/>
-    <row r="598" s="32" customFormat="1" ht="12.75"/>
-    <row r="599" s="32" customFormat="1" ht="12.75"/>
-    <row r="600" s="32" customFormat="1" ht="12.75"/>
-    <row r="601" s="32" customFormat="1" ht="12.75"/>
-    <row r="602" s="32" customFormat="1" ht="12.75"/>
-    <row r="603" s="32" customFormat="1" ht="12.75"/>
-    <row r="604" s="32" customFormat="1" ht="12.75"/>
-    <row r="605" s="32" customFormat="1" ht="12.75"/>
-    <row r="606" s="32" customFormat="1" ht="12.75"/>
-    <row r="607" s="32" customFormat="1" ht="12.75"/>
-    <row r="608" s="32" customFormat="1" ht="12.75"/>
-    <row r="609" s="32" customFormat="1" ht="12.75"/>
-    <row r="610" s="32" customFormat="1" ht="12.75"/>
-    <row r="611" s="32" customFormat="1" ht="12.75"/>
-    <row r="612" s="32" customFormat="1" ht="12.75"/>
-    <row r="613" s="32" customFormat="1" ht="12.75"/>
-    <row r="614" s="32" customFormat="1" ht="12.75"/>
-    <row r="615" s="32" customFormat="1" ht="12.75"/>
-    <row r="616" s="32" customFormat="1" ht="12.75"/>
-    <row r="617" s="32" customFormat="1" ht="12.75"/>
-    <row r="618" s="32" customFormat="1" ht="12.75"/>
-    <row r="619" s="32" customFormat="1" ht="12.75"/>
-    <row r="620" s="32" customFormat="1" ht="12.75"/>
-    <row r="621" s="32" customFormat="1" ht="12.75"/>
-    <row r="622" s="32" customFormat="1" ht="12.75"/>
-    <row r="623" s="32" customFormat="1" ht="12.75"/>
-    <row r="624" s="32" customFormat="1" ht="12.75"/>
-    <row r="625" s="32" customFormat="1" ht="12.75"/>
-    <row r="626" s="32" customFormat="1" ht="12.75"/>
-    <row r="627" s="32" customFormat="1" ht="12.75"/>
-    <row r="628" s="32" customFormat="1" ht="12.75"/>
-    <row r="629" s="32" customFormat="1" ht="12.75"/>
-    <row r="630" s="32" customFormat="1" ht="12.75"/>
-    <row r="631" s="32" customFormat="1" ht="12.75"/>
-    <row r="632" s="32" customFormat="1" ht="12.75"/>
-    <row r="633" s="32" customFormat="1" ht="12.75"/>
-    <row r="634" s="32" customFormat="1" ht="12.75"/>
-    <row r="635" s="32" customFormat="1" ht="12.75"/>
-    <row r="636" s="32" customFormat="1" ht="12.75"/>
-    <row r="637" s="32" customFormat="1" ht="12.75"/>
-    <row r="638" s="32" customFormat="1" ht="12.75"/>
-    <row r="639" s="32" customFormat="1" ht="12.75"/>
-    <row r="640" s="32" customFormat="1" ht="12.75"/>
-    <row r="641" s="32" customFormat="1" ht="12.75"/>
-    <row r="642" s="32" customFormat="1" ht="12.75"/>
-    <row r="643" s="32" customFormat="1" ht="12.75"/>
-    <row r="644" s="32" customFormat="1" ht="12.75"/>
-    <row r="645" s="32" customFormat="1" ht="12.75"/>
-    <row r="646" s="32" customFormat="1" ht="12.75"/>
-    <row r="647" s="32" customFormat="1" ht="12.75"/>
-    <row r="648" s="32" customFormat="1" ht="12.75"/>
-    <row r="649" s="32" customFormat="1" ht="12.75"/>
-    <row r="650" s="32" customFormat="1" ht="12.75"/>
-    <row r="651" s="32" customFormat="1" ht="12.75"/>
-    <row r="652" s="32" customFormat="1" ht="12.75"/>
-    <row r="653" s="32" customFormat="1" ht="12.75"/>
-    <row r="654" s="32" customFormat="1" ht="12.75"/>
-    <row r="655" s="32" customFormat="1" ht="12.75"/>
-    <row r="656" s="32" customFormat="1" ht="12.75"/>
-    <row r="657" s="32" customFormat="1" ht="12.75"/>
-    <row r="658" s="32" customFormat="1" ht="12.75"/>
-    <row r="659" s="32" customFormat="1" ht="12.75"/>
-    <row r="660" s="32" customFormat="1" ht="12.75"/>
-    <row r="661" s="32" customFormat="1" ht="12.75"/>
-    <row r="662" s="32" customFormat="1" ht="12.75"/>
-    <row r="663" s="32" customFormat="1" ht="12.75"/>
-    <row r="664" s="32" customFormat="1" ht="12.75"/>
-    <row r="665" s="32" customFormat="1" ht="12.75"/>
-    <row r="666" s="32" customFormat="1" ht="12.75"/>
-    <row r="667" s="32" customFormat="1" ht="12.75"/>
-    <row r="668" s="32" customFormat="1" ht="12.75"/>
-    <row r="669" s="32" customFormat="1" ht="12.75"/>
-    <row r="670" s="32" customFormat="1" ht="12.75"/>
-    <row r="671" s="32" customFormat="1" ht="12.75"/>
-    <row r="672" s="32" customFormat="1" ht="12.75"/>
-    <row r="673" s="32" customFormat="1" ht="12.75"/>
-    <row r="674" s="32" customFormat="1" ht="12.75"/>
-    <row r="675" s="32" customFormat="1" ht="12.75"/>
-    <row r="676" s="32" customFormat="1" ht="12.75"/>
-    <row r="677" s="32" customFormat="1" ht="12.75"/>
-    <row r="678" s="32" customFormat="1" ht="12.75"/>
-    <row r="679" s="32" customFormat="1" ht="12.75"/>
-    <row r="680" s="32" customFormat="1" ht="12.75"/>
-    <row r="681" s="32" customFormat="1" ht="12.75"/>
-    <row r="682" s="32" customFormat="1" ht="12.75"/>
-    <row r="683" s="32" customFormat="1" ht="12.75"/>
-    <row r="684" s="32" customFormat="1" ht="12.75"/>
-    <row r="685" s="32" customFormat="1" ht="12.75"/>
-    <row r="686" s="32" customFormat="1" ht="12.75"/>
-    <row r="687" s="32" customFormat="1" ht="12.75"/>
-    <row r="688" s="32" customFormat="1" ht="12.75"/>
-    <row r="689" s="32" customFormat="1" ht="12.75"/>
-    <row r="690" s="32" customFormat="1" ht="12.75"/>
-    <row r="691" s="32" customFormat="1" ht="12.75"/>
-    <row r="692" s="32" customFormat="1" ht="12.75"/>
-    <row r="693" s="32" customFormat="1" ht="12.75"/>
-    <row r="694" s="32" customFormat="1" ht="12.75"/>
-    <row r="695" s="32" customFormat="1" ht="12.75"/>
-    <row r="696" s="32" customFormat="1" ht="12.75"/>
-    <row r="697" s="32" customFormat="1" ht="12.75"/>
-    <row r="698" s="32" customFormat="1" ht="12.75"/>
-    <row r="699" s="32" customFormat="1" ht="12.75"/>
-    <row r="700" s="32" customFormat="1" ht="12.75"/>
-    <row r="701" s="32" customFormat="1" ht="12.75"/>
-    <row r="702" s="32" customFormat="1" ht="12.75"/>
-    <row r="703" s="32" customFormat="1" ht="12.75"/>
-    <row r="704" s="32" customFormat="1" ht="12.75"/>
-    <row r="705" s="32" customFormat="1" ht="12.75"/>
-    <row r="706" s="32" customFormat="1" ht="12.75"/>
-    <row r="707" s="32" customFormat="1" ht="12.75"/>
-    <row r="708" s="32" customFormat="1" ht="12.75"/>
-    <row r="709" s="32" customFormat="1" ht="12.75"/>
-    <row r="710" s="32" customFormat="1" ht="12.75"/>
-    <row r="711" s="32" customFormat="1" ht="12.75"/>
-    <row r="712" s="32" customFormat="1" ht="12.75"/>
-    <row r="713" s="32" customFormat="1" ht="12.75"/>
-    <row r="714" s="32" customFormat="1" ht="12.75"/>
-    <row r="715" s="32" customFormat="1" ht="12.75"/>
-    <row r="716" s="32" customFormat="1" ht="12.75"/>
-    <row r="717" s="32" customFormat="1" ht="12.75"/>
-    <row r="718" s="32" customFormat="1" ht="12.75"/>
-    <row r="719" s="32" customFormat="1" ht="12.75"/>
-    <row r="720" s="32" customFormat="1" ht="12.75"/>
-    <row r="721" s="32" customFormat="1" ht="12.75"/>
-    <row r="722" s="32" customFormat="1" ht="12.75"/>
-    <row r="723" s="32" customFormat="1" ht="12.75"/>
-    <row r="724" s="32" customFormat="1" ht="12.75"/>
-    <row r="725" s="32" customFormat="1" ht="12.75"/>
-    <row r="726" s="32" customFormat="1" ht="12.75"/>
-    <row r="727" s="32" customFormat="1" ht="12.75"/>
-    <row r="728" s="32" customFormat="1" ht="12.75"/>
-    <row r="729" s="32" customFormat="1" ht="12.75"/>
-    <row r="730" s="32" customFormat="1" ht="12.75"/>
-    <row r="731" s="32" customFormat="1" ht="12.75"/>
-    <row r="732" s="32" customFormat="1" ht="12.75"/>
-    <row r="733" s="32" customFormat="1" ht="12.75"/>
-    <row r="734" s="32" customFormat="1" ht="12.75"/>
-    <row r="735" s="32" customFormat="1" ht="12.75"/>
-    <row r="736" s="32" customFormat="1" ht="12.75"/>
-    <row r="737" s="32" customFormat="1" ht="12.75"/>
-    <row r="738" s="32" customFormat="1" ht="12.75"/>
-    <row r="739" s="32" customFormat="1" ht="12.75"/>
-    <row r="740" s="32" customFormat="1" ht="12.75"/>
-    <row r="741" s="32" customFormat="1" ht="12.75"/>
-    <row r="742" s="32" customFormat="1" ht="12.75"/>
-    <row r="743" s="32" customFormat="1" ht="12.75"/>
-    <row r="744" s="32" customFormat="1" ht="12.75"/>
-    <row r="745" s="32" customFormat="1" ht="12.75"/>
-    <row r="746" s="32" customFormat="1" ht="12.75"/>
-    <row r="747" s="32" customFormat="1" ht="12.75"/>
-    <row r="748" s="32" customFormat="1" ht="12.75"/>
-    <row r="749" s="32" customFormat="1" ht="12.75"/>
-    <row r="750" s="32" customFormat="1" ht="12.75"/>
-    <row r="751" s="32" customFormat="1" ht="12.75"/>
-    <row r="752" s="32" customFormat="1" ht="12.75"/>
-    <row r="753" s="32" customFormat="1" ht="12.75"/>
-    <row r="754" s="32" customFormat="1" ht="12.75"/>
-    <row r="755" s="32" customFormat="1" ht="12.75"/>
-    <row r="756" s="32" customFormat="1" ht="12.75"/>
-    <row r="757" s="32" customFormat="1" ht="12.75"/>
-    <row r="758" s="32" customFormat="1" ht="12.75"/>
-    <row r="759" s="32" customFormat="1" ht="12.75"/>
-    <row r="760" s="32" customFormat="1" ht="12.75"/>
-    <row r="761" s="32" customFormat="1" ht="12.75"/>
-    <row r="762" s="32" customFormat="1" ht="12.75"/>
-    <row r="763" s="32" customFormat="1" ht="12.75"/>
-    <row r="764" s="32" customFormat="1" ht="12.75"/>
-    <row r="765" s="32" customFormat="1" ht="12.75"/>
-    <row r="766" s="32" customFormat="1" ht="12.75"/>
-    <row r="767" s="32" customFormat="1" ht="12.75"/>
-    <row r="768" s="32" customFormat="1" ht="12.75"/>
-    <row r="769" s="32" customFormat="1" ht="12.75"/>
-    <row r="770" s="32" customFormat="1" ht="12.75"/>
-    <row r="771" s="32" customFormat="1" ht="12.75"/>
-    <row r="772" s="32" customFormat="1" ht="12.75"/>
-    <row r="773" s="32" customFormat="1" ht="12.75"/>
-    <row r="774" s="32" customFormat="1" ht="12.75"/>
-    <row r="775" s="32" customFormat="1" ht="12.75"/>
-    <row r="776" s="32" customFormat="1" ht="12.75"/>
-    <row r="777" s="32" customFormat="1" ht="12.75"/>
-    <row r="778" s="32" customFormat="1" ht="12.75"/>
-    <row r="779" s="32" customFormat="1" ht="12.75"/>
-    <row r="780" s="32" customFormat="1" ht="12.75"/>
-    <row r="781" s="32" customFormat="1" ht="12.75"/>
-    <row r="782" s="32" customFormat="1" ht="12.75"/>
-    <row r="783" s="32" customFormat="1" ht="12.75"/>
-    <row r="784" s="32" customFormat="1" ht="12.75"/>
-    <row r="785" s="32" customFormat="1" ht="12.75"/>
-    <row r="786" s="32" customFormat="1" ht="12.75"/>
-    <row r="787" s="32" customFormat="1" ht="12.75"/>
-    <row r="788" s="32" customFormat="1" ht="12.75"/>
-    <row r="789" s="32" customFormat="1" ht="12.75"/>
-    <row r="790" s="32" customFormat="1" ht="12.75"/>
-    <row r="791" s="32" customFormat="1" ht="12.75"/>
-    <row r="792" s="32" customFormat="1" ht="12.75"/>
-    <row r="793" s="32" customFormat="1" ht="12.75"/>
-    <row r="794" s="32" customFormat="1" ht="12.75"/>
-    <row r="795" s="32" customFormat="1" ht="12.75"/>
-    <row r="796" s="32" customFormat="1" ht="12.75"/>
-    <row r="797" s="32" customFormat="1" ht="12.75"/>
-    <row r="798" s="32" customFormat="1" ht="12.75"/>
-    <row r="799" s="32" customFormat="1" ht="12.75"/>
-    <row r="800" s="32" customFormat="1" ht="12.75"/>
-    <row r="801" s="32" customFormat="1" ht="12.75"/>
-    <row r="802" s="32" customFormat="1" ht="12.75"/>
-    <row r="803" s="32" customFormat="1" ht="12.75"/>
-    <row r="804" s="32" customFormat="1" ht="12.75"/>
-    <row r="805" s="32" customFormat="1" ht="12.75"/>
-    <row r="806" s="32" customFormat="1" ht="12.75"/>
-    <row r="807" s="32" customFormat="1" ht="12.75"/>
-    <row r="808" s="32" customFormat="1" ht="12.75"/>
-    <row r="809" s="32" customFormat="1" ht="12.75"/>
-    <row r="810" s="32" customFormat="1" ht="12.75"/>
-    <row r="811" s="32" customFormat="1" ht="12.75"/>
-    <row r="812" s="32" customFormat="1" ht="12.75"/>
-    <row r="813" s="32" customFormat="1" ht="12.75"/>
-    <row r="814" s="32" customFormat="1" ht="12.75"/>
-    <row r="815" s="32" customFormat="1" ht="12.75"/>
-    <row r="816" s="32" customFormat="1" ht="12.75"/>
-    <row r="817" s="32" customFormat="1" ht="12.75"/>
-    <row r="818" s="32" customFormat="1" ht="12.75"/>
-    <row r="819" s="32" customFormat="1" ht="12.75"/>
-    <row r="820" s="32" customFormat="1" ht="12.75"/>
-    <row r="821" s="32" customFormat="1" ht="12.75"/>
-    <row r="822" s="32" customFormat="1" ht="12.75"/>
-    <row r="823" s="32" customFormat="1" ht="12.75"/>
-    <row r="824" s="32" customFormat="1" ht="12.75"/>
-    <row r="825" s="32" customFormat="1" ht="12.75"/>
-    <row r="826" s="32" customFormat="1" ht="12.75"/>
-    <row r="827" s="32" customFormat="1" ht="12.75"/>
-    <row r="828" s="32" customFormat="1" ht="12.75"/>
-    <row r="829" s="32" customFormat="1" ht="12.75"/>
-    <row r="830" s="32" customFormat="1" ht="12.75"/>
-    <row r="831" s="32" customFormat="1" ht="12.75"/>
-    <row r="832" s="32" customFormat="1" ht="12.75"/>
-    <row r="833" s="32" customFormat="1" ht="12.75"/>
-    <row r="834" s="32" customFormat="1" ht="12.75"/>
-    <row r="835" s="32" customFormat="1" ht="12.75"/>
-    <row r="836" s="32" customFormat="1" ht="12.75"/>
-    <row r="837" s="32" customFormat="1" ht="12.75"/>
-    <row r="838" s="32" customFormat="1" ht="12.75"/>
-    <row r="839" s="32" customFormat="1" ht="12.75"/>
-    <row r="840" s="32" customFormat="1" ht="12.75"/>
-    <row r="841" s="32" customFormat="1" ht="12.75"/>
-    <row r="842" s="32" customFormat="1" ht="12.75"/>
-    <row r="843" s="32" customFormat="1" ht="12.75"/>
-    <row r="844" s="32" customFormat="1" ht="12.75"/>
-    <row r="845" s="32" customFormat="1" ht="12.75"/>
-    <row r="846" s="32" customFormat="1" ht="12.75"/>
-    <row r="847" s="32" customFormat="1" ht="12.75"/>
-    <row r="848" s="32" customFormat="1" ht="12.75"/>
-    <row r="849" s="32" customFormat="1" ht="12.75"/>
-    <row r="850" s="32" customFormat="1" ht="12.75"/>
-    <row r="851" s="32" customFormat="1" ht="12.75"/>
-    <row r="852" s="32" customFormat="1" ht="12.75"/>
-    <row r="853" s="32" customFormat="1" ht="12.75"/>
-    <row r="854" s="32" customFormat="1" ht="12.75"/>
-    <row r="855" s="32" customFormat="1" ht="12.75"/>
-    <row r="856" s="32" customFormat="1" ht="12.75"/>
-    <row r="857" s="32" customFormat="1" ht="12.75"/>
-    <row r="858" s="32" customFormat="1" ht="12.75"/>
-    <row r="859" s="32" customFormat="1" ht="12.75"/>
-    <row r="860" s="32" customFormat="1" ht="12.75"/>
-    <row r="861" s="32" customFormat="1" ht="12.75"/>
-    <row r="862" s="32" customFormat="1" ht="12.75"/>
-    <row r="863" s="32" customFormat="1" ht="12.75"/>
-    <row r="864" s="32" customFormat="1" ht="12.75"/>
-    <row r="865" s="32" customFormat="1" ht="12.75"/>
-    <row r="866" s="32" customFormat="1" ht="12.75"/>
-    <row r="867" s="32" customFormat="1" ht="12.75"/>
-    <row r="868" s="32" customFormat="1" ht="12.75"/>
-    <row r="869" s="32" customFormat="1" ht="12.75"/>
-    <row r="870" s="32" customFormat="1" ht="12.75"/>
-    <row r="871" s="32" customFormat="1" ht="12.75"/>
-    <row r="872" s="32" customFormat="1" ht="12.75"/>
-    <row r="873" s="32" customFormat="1" ht="12.75"/>
-    <row r="874" s="32" customFormat="1" ht="12.75"/>
-    <row r="875" s="32" customFormat="1" ht="12.75"/>
-    <row r="876" s="32" customFormat="1" ht="12.75"/>
-    <row r="877" s="32" customFormat="1" ht="12.75"/>
-    <row r="878" s="32" customFormat="1" ht="12.75"/>
-    <row r="879" s="32" customFormat="1" ht="12.75"/>
-    <row r="880" s="32" customFormat="1" ht="12.75"/>
-    <row r="881" s="32" customFormat="1" ht="12.75"/>
-    <row r="882" s="32" customFormat="1" ht="12.75"/>
-    <row r="883" s="32" customFormat="1" ht="12.75"/>
-    <row r="884" s="32" customFormat="1" ht="12.75"/>
-    <row r="885" s="32" customFormat="1" ht="12.75"/>
-    <row r="886" s="32" customFormat="1" ht="12.75"/>
-    <row r="887" s="32" customFormat="1" ht="12.75"/>
-    <row r="888" s="32" customFormat="1" ht="12.75"/>
-    <row r="889" s="32" customFormat="1" ht="12.75"/>
-    <row r="890" s="32" customFormat="1" ht="12.75"/>
-    <row r="891" s="32" customFormat="1" ht="12.75"/>
-    <row r="892" s="32" customFormat="1" ht="12.75"/>
-    <row r="893" s="32" customFormat="1" ht="12.75"/>
-    <row r="894" s="32" customFormat="1" ht="12.75"/>
-    <row r="895" s="32" customFormat="1" ht="12.75"/>
-    <row r="896" s="32" customFormat="1" ht="12.75"/>
-    <row r="897" s="32" customFormat="1" ht="12.75"/>
-    <row r="898" s="32" customFormat="1" ht="12.75"/>
-    <row r="899" s="32" customFormat="1" ht="12.75"/>
-    <row r="900" s="32" customFormat="1" ht="12.75"/>
-    <row r="901" s="32" customFormat="1" ht="12.75"/>
-    <row r="902" s="32" customFormat="1" ht="12.75"/>
-    <row r="903" s="32" customFormat="1" ht="12.75"/>
-    <row r="904" s="32" customFormat="1" ht="12.75"/>
-    <row r="905" s="32" customFormat="1" ht="12.75"/>
-    <row r="906" s="32" customFormat="1" ht="12.75"/>
-    <row r="907" s="32" customFormat="1" ht="12.75"/>
-    <row r="908" s="32" customFormat="1" ht="12.75"/>
-    <row r="909" s="32" customFormat="1" ht="12.75"/>
-    <row r="910" s="32" customFormat="1" ht="12.75"/>
-    <row r="911" s="32" customFormat="1" ht="12.75"/>
-    <row r="912" s="32" customFormat="1" ht="12.75"/>
-    <row r="913" s="32" customFormat="1" ht="12.75"/>
-    <row r="914" s="32" customFormat="1" ht="12.75"/>
-    <row r="915" s="32" customFormat="1" ht="12.75"/>
-    <row r="916" s="32" customFormat="1" ht="12.75"/>
-    <row r="917" s="32" customFormat="1" ht="12.75"/>
-    <row r="918" s="32" customFormat="1" ht="12.75"/>
-    <row r="919" s="32" customFormat="1" ht="12.75"/>
-    <row r="920" s="32" customFormat="1" ht="12.75"/>
-    <row r="921" s="32" customFormat="1" ht="12.75"/>
-    <row r="922" s="32" customFormat="1" ht="12.75"/>
-    <row r="923" s="32" customFormat="1" ht="12.75"/>
-    <row r="924" s="32" customFormat="1" ht="12.75"/>
-    <row r="925" s="32" customFormat="1" ht="12.75"/>
-    <row r="926" s="32" customFormat="1" ht="12.75"/>
-    <row r="927" s="32" customFormat="1" ht="12.75"/>
-    <row r="928" s="32" customFormat="1" ht="12.75"/>
-    <row r="929" s="32" customFormat="1" ht="12.75"/>
-    <row r="930" s="32" customFormat="1" ht="12.75"/>
-    <row r="931" s="32" customFormat="1" ht="12.75"/>
-    <row r="932" s="32" customFormat="1" ht="12.75"/>
-    <row r="933" s="32" customFormat="1" ht="12.75"/>
-    <row r="934" s="32" customFormat="1" ht="12.75"/>
-    <row r="935" s="32" customFormat="1" ht="12.75"/>
-    <row r="936" s="32" customFormat="1" ht="12.75"/>
-    <row r="937" s="32" customFormat="1" ht="12.75"/>
-    <row r="938" s="32" customFormat="1" ht="12.75"/>
-    <row r="939" s="32" customFormat="1" ht="12.75"/>
-    <row r="940" s="32" customFormat="1" ht="12.75"/>
-    <row r="941" s="32" customFormat="1" ht="12.75"/>
-    <row r="942" s="32" customFormat="1" ht="12.75"/>
-    <row r="943" s="32" customFormat="1" ht="12.75"/>
-    <row r="944" s="32" customFormat="1" ht="12.75"/>
-    <row r="945" s="32" customFormat="1" ht="12.75"/>
-    <row r="946" s="32" customFormat="1" ht="12.75"/>
-    <row r="947" s="32" customFormat="1" ht="12.75"/>
-    <row r="948" s="32" customFormat="1" ht="12.75"/>
-    <row r="949" s="32" customFormat="1" ht="12.75"/>
-    <row r="950" s="32" customFormat="1" ht="12.75"/>
-    <row r="951" s="32" customFormat="1" ht="12.75"/>
-    <row r="952" s="32" customFormat="1" ht="12.75"/>
-    <row r="953" s="32" customFormat="1" ht="12.75"/>
-    <row r="954" s="32" customFormat="1" ht="12.75"/>
-    <row r="955" s="32" customFormat="1" ht="12.75"/>
-    <row r="956" s="32" customFormat="1" ht="12.75"/>
-    <row r="957" s="32" customFormat="1" ht="12.75"/>
-    <row r="958" s="32" customFormat="1" ht="12.75"/>
-    <row r="959" s="32" customFormat="1" ht="12.75"/>
-    <row r="960" s="32" customFormat="1" ht="12.75"/>
-    <row r="961" s="32" customFormat="1" ht="12.75"/>
-    <row r="962" s="32" customFormat="1" ht="12.75"/>
-    <row r="963" s="32" customFormat="1" ht="12.75"/>
-    <row r="964" s="32" customFormat="1" ht="12.75"/>
-    <row r="965" s="32" customFormat="1" ht="12.75"/>
-    <row r="966" s="32" customFormat="1" ht="12.75"/>
-    <row r="967" s="32" customFormat="1" ht="12.75"/>
-    <row r="968" s="32" customFormat="1" ht="12.75"/>
-    <row r="969" s="32" customFormat="1" ht="12.75"/>
-    <row r="970" s="32" customFormat="1" ht="12.75"/>
-    <row r="971" s="32" customFormat="1" ht="12.75"/>
-    <row r="972" s="32" customFormat="1" ht="12.75"/>
-    <row r="973" s="32" customFormat="1" ht="12.75"/>
-    <row r="974" s="32" customFormat="1" ht="12.75"/>
-    <row r="975" s="32" customFormat="1" ht="12.75"/>
-    <row r="976" s="32" customFormat="1" ht="12.75"/>
-    <row r="977" s="32" customFormat="1" ht="12.75"/>
-    <row r="978" s="32" customFormat="1" ht="12.75"/>
-    <row r="979" s="32" customFormat="1" ht="12.75"/>
-    <row r="980" s="32" customFormat="1" ht="12.75"/>
-    <row r="981" s="32" customFormat="1" ht="12.75"/>
-    <row r="982" s="32" customFormat="1" ht="12.75"/>
-    <row r="983" s="32" customFormat="1" ht="12.75"/>
-    <row r="984" s="32" customFormat="1" ht="12.75"/>
-    <row r="985" s="32" customFormat="1" ht="12.75"/>
-    <row r="986" s="32" customFormat="1" ht="12.75"/>
-    <row r="987" s="32" customFormat="1" ht="12.75"/>
+    <row r="17" s="30" customFormat="1" ht="12.75"/>
+    <row r="18" s="30" customFormat="1" ht="12.75"/>
+    <row r="19" s="30" customFormat="1" ht="12.75"/>
+    <row r="20" s="30" customFormat="1" ht="12.75"/>
+    <row r="21" s="30" customFormat="1" ht="12.75"/>
+    <row r="22" s="30" customFormat="1" ht="12.75"/>
+    <row r="23" s="30" customFormat="1" ht="12.75"/>
+    <row r="24" s="30" customFormat="1" ht="12.75"/>
+    <row r="25" s="30" customFormat="1" ht="12.75"/>
+    <row r="26" s="30" customFormat="1" ht="12.75"/>
+    <row r="27" s="30" customFormat="1" ht="12.75"/>
+    <row r="28" s="30" customFormat="1" ht="12.75"/>
+    <row r="29" s="30" customFormat="1" ht="12.75"/>
+    <row r="30" s="30" customFormat="1" ht="12.75"/>
+    <row r="31" s="30" customFormat="1" ht="12.75"/>
+    <row r="32" s="30" customFormat="1" ht="12.75"/>
+    <row r="33" s="30" customFormat="1" ht="12.75"/>
+    <row r="34" s="30" customFormat="1" ht="12.75"/>
+    <row r="35" s="30" customFormat="1" ht="12.75"/>
+    <row r="36" s="30" customFormat="1" ht="12.75"/>
+    <row r="37" s="30" customFormat="1" ht="12.75"/>
+    <row r="38" s="30" customFormat="1" ht="12.75"/>
+    <row r="39" s="30" customFormat="1" ht="12.75"/>
+    <row r="40" s="30" customFormat="1" ht="12.75"/>
+    <row r="41" s="30" customFormat="1" ht="12.75"/>
+    <row r="42" s="30" customFormat="1" ht="12.75"/>
+    <row r="43" s="30" customFormat="1" ht="12.75"/>
+    <row r="44" s="30" customFormat="1" ht="12.75"/>
+    <row r="45" s="30" customFormat="1" ht="12.75"/>
+    <row r="46" s="30" customFormat="1" ht="12.75"/>
+    <row r="47" s="30" customFormat="1" ht="12.75"/>
+    <row r="48" s="30" customFormat="1" ht="12.75"/>
+    <row r="49" s="30" customFormat="1" ht="12.75"/>
+    <row r="50" s="30" customFormat="1" ht="12.75"/>
+    <row r="51" s="30" customFormat="1" ht="12.75"/>
+    <row r="52" s="30" customFormat="1" ht="12.75"/>
+    <row r="53" s="30" customFormat="1" ht="12.75"/>
+    <row r="54" s="30" customFormat="1" ht="12.75"/>
+    <row r="55" s="30" customFormat="1" ht="12.75"/>
+    <row r="56" s="30" customFormat="1" ht="12.75"/>
+    <row r="57" s="30" customFormat="1" ht="12.75"/>
+    <row r="58" s="30" customFormat="1" ht="12.75"/>
+    <row r="59" s="30" customFormat="1" ht="12.75"/>
+    <row r="60" s="30" customFormat="1" ht="12.75"/>
+    <row r="61" s="30" customFormat="1" ht="12.75"/>
+    <row r="62" s="30" customFormat="1" ht="12.75"/>
+    <row r="63" s="30" customFormat="1" ht="12.75"/>
+    <row r="64" s="30" customFormat="1" ht="12.75"/>
+    <row r="65" s="30" customFormat="1" ht="12.75"/>
+    <row r="66" s="30" customFormat="1" ht="12.75"/>
+    <row r="67" s="30" customFormat="1" ht="12.75"/>
+    <row r="68" s="30" customFormat="1" ht="12.75"/>
+    <row r="69" s="30" customFormat="1" ht="12.75"/>
+    <row r="70" s="30" customFormat="1" ht="12.75"/>
+    <row r="71" s="30" customFormat="1" ht="12.75"/>
+    <row r="72" s="30" customFormat="1" ht="12.75"/>
+    <row r="73" s="30" customFormat="1" ht="12.75"/>
+    <row r="74" s="30" customFormat="1" ht="12.75"/>
+    <row r="75" s="30" customFormat="1" ht="12.75"/>
+    <row r="76" s="30" customFormat="1" ht="12.75"/>
+    <row r="77" s="30" customFormat="1" ht="12.75"/>
+    <row r="78" s="30" customFormat="1" ht="12.75"/>
+    <row r="79" s="30" customFormat="1" ht="12.75"/>
+    <row r="80" s="30" customFormat="1" ht="12.75"/>
+    <row r="81" s="30" customFormat="1" ht="12.75"/>
+    <row r="82" s="30" customFormat="1" ht="12.75"/>
+    <row r="83" s="30" customFormat="1" ht="12.75"/>
+    <row r="84" s="30" customFormat="1" ht="12.75"/>
+    <row r="85" s="30" customFormat="1" ht="12.75"/>
+    <row r="86" s="30" customFormat="1" ht="12.75"/>
+    <row r="87" s="30" customFormat="1" ht="12.75"/>
+    <row r="88" s="30" customFormat="1" ht="12.75"/>
+    <row r="89" s="30" customFormat="1" ht="12.75"/>
+    <row r="90" s="30" customFormat="1" ht="12.75"/>
+    <row r="91" s="30" customFormat="1" ht="12.75"/>
+    <row r="92" s="30" customFormat="1" ht="12.75"/>
+    <row r="93" s="30" customFormat="1" ht="12.75"/>
+    <row r="94" s="30" customFormat="1" ht="12.75"/>
+    <row r="95" s="30" customFormat="1" ht="12.75"/>
+    <row r="96" s="30" customFormat="1" ht="12.75"/>
+    <row r="97" s="30" customFormat="1" ht="12.75"/>
+    <row r="98" s="30" customFormat="1" ht="12.75"/>
+    <row r="99" s="30" customFormat="1" ht="12.75"/>
+    <row r="100" s="30" customFormat="1" ht="12.75"/>
+    <row r="101" s="30" customFormat="1" ht="12.75"/>
+    <row r="102" s="30" customFormat="1" ht="12.75"/>
+    <row r="103" s="30" customFormat="1" ht="12.75"/>
+    <row r="104" s="30" customFormat="1" ht="12.75"/>
+    <row r="105" s="30" customFormat="1" ht="12.75"/>
+    <row r="106" s="30" customFormat="1" ht="12.75"/>
+    <row r="107" s="30" customFormat="1" ht="12.75"/>
+    <row r="108" s="30" customFormat="1" ht="12.75"/>
+    <row r="109" s="30" customFormat="1" ht="12.75"/>
+    <row r="110" s="30" customFormat="1" ht="12.75"/>
+    <row r="111" s="30" customFormat="1" ht="12.75"/>
+    <row r="112" s="30" customFormat="1" ht="12.75"/>
+    <row r="113" s="30" customFormat="1" ht="12.75"/>
+    <row r="114" s="30" customFormat="1" ht="12.75"/>
+    <row r="115" s="30" customFormat="1" ht="12.75"/>
+    <row r="116" s="30" customFormat="1" ht="12.75"/>
+    <row r="117" s="30" customFormat="1" ht="12.75"/>
+    <row r="118" s="30" customFormat="1" ht="12.75"/>
+    <row r="119" s="30" customFormat="1" ht="12.75"/>
+    <row r="120" s="30" customFormat="1" ht="12.75"/>
+    <row r="121" s="30" customFormat="1" ht="12.75"/>
+    <row r="122" s="30" customFormat="1" ht="12.75"/>
+    <row r="123" s="30" customFormat="1" ht="12.75"/>
+    <row r="124" s="30" customFormat="1" ht="12.75"/>
+    <row r="125" s="30" customFormat="1" ht="12.75"/>
+    <row r="126" s="30" customFormat="1" ht="12.75"/>
+    <row r="127" s="30" customFormat="1" ht="12.75"/>
+    <row r="128" s="30" customFormat="1" ht="12.75"/>
+    <row r="129" s="30" customFormat="1" ht="12.75"/>
+    <row r="130" s="30" customFormat="1" ht="12.75"/>
+    <row r="131" s="30" customFormat="1" ht="12.75"/>
+    <row r="132" s="30" customFormat="1" ht="12.75"/>
+    <row r="133" s="30" customFormat="1" ht="12.75"/>
+    <row r="134" s="30" customFormat="1" ht="12.75"/>
+    <row r="135" s="30" customFormat="1" ht="12.75"/>
+    <row r="136" s="30" customFormat="1" ht="12.75"/>
+    <row r="137" s="30" customFormat="1" ht="12.75"/>
+    <row r="138" s="30" customFormat="1" ht="12.75"/>
+    <row r="139" s="30" customFormat="1" ht="12.75"/>
+    <row r="140" s="30" customFormat="1" ht="12.75"/>
+    <row r="141" s="30" customFormat="1" ht="12.75"/>
+    <row r="142" s="30" customFormat="1" ht="12.75"/>
+    <row r="143" s="30" customFormat="1" ht="12.75"/>
+    <row r="144" s="30" customFormat="1" ht="12.75"/>
+    <row r="145" s="30" customFormat="1" ht="12.75"/>
+    <row r="146" s="30" customFormat="1" ht="12.75"/>
+    <row r="147" s="30" customFormat="1" ht="12.75"/>
+    <row r="148" s="30" customFormat="1" ht="12.75"/>
+    <row r="149" s="30" customFormat="1" ht="12.75"/>
+    <row r="150" s="30" customFormat="1" ht="12.75"/>
+    <row r="151" s="30" customFormat="1" ht="12.75"/>
+    <row r="152" s="30" customFormat="1" ht="12.75"/>
+    <row r="153" s="30" customFormat="1" ht="12.75"/>
+    <row r="154" s="30" customFormat="1" ht="12.75"/>
+    <row r="155" s="30" customFormat="1" ht="12.75"/>
+    <row r="156" s="30" customFormat="1" ht="12.75"/>
+    <row r="157" s="30" customFormat="1" ht="12.75"/>
+    <row r="158" s="30" customFormat="1" ht="12.75"/>
+    <row r="159" s="30" customFormat="1" ht="12.75"/>
+    <row r="160" s="30" customFormat="1" ht="12.75"/>
+    <row r="161" s="30" customFormat="1" ht="12.75"/>
+    <row r="162" s="30" customFormat="1" ht="12.75"/>
+    <row r="163" s="30" customFormat="1" ht="12.75"/>
+    <row r="164" s="30" customFormat="1" ht="12.75"/>
+    <row r="165" s="30" customFormat="1" ht="12.75"/>
+    <row r="166" s="30" customFormat="1" ht="12.75"/>
+    <row r="167" s="30" customFormat="1" ht="12.75"/>
+    <row r="168" s="30" customFormat="1" ht="12.75"/>
+    <row r="169" s="30" customFormat="1" ht="12.75"/>
+    <row r="170" s="30" customFormat="1" ht="12.75"/>
+    <row r="171" s="30" customFormat="1" ht="12.75"/>
+    <row r="172" s="30" customFormat="1" ht="12.75"/>
+    <row r="173" s="30" customFormat="1" ht="12.75"/>
+    <row r="174" s="30" customFormat="1" ht="12.75"/>
+    <row r="175" s="30" customFormat="1" ht="12.75"/>
+    <row r="176" s="30" customFormat="1" ht="12.75"/>
+    <row r="177" s="30" customFormat="1" ht="12.75"/>
+    <row r="178" s="30" customFormat="1" ht="12.75"/>
+    <row r="179" s="30" customFormat="1" ht="12.75"/>
+    <row r="180" s="30" customFormat="1" ht="12.75"/>
+    <row r="181" s="30" customFormat="1" ht="12.75"/>
+    <row r="182" s="30" customFormat="1" ht="12.75"/>
+    <row r="183" s="30" customFormat="1" ht="12.75"/>
+    <row r="184" s="30" customFormat="1" ht="12.75"/>
+    <row r="185" s="30" customFormat="1" ht="12.75"/>
+    <row r="186" s="30" customFormat="1" ht="12.75"/>
+    <row r="187" s="30" customFormat="1" ht="12.75"/>
+    <row r="188" s="30" customFormat="1" ht="12.75"/>
+    <row r="189" s="30" customFormat="1" ht="12.75"/>
+    <row r="190" s="30" customFormat="1" ht="12.75"/>
+    <row r="191" s="30" customFormat="1" ht="12.75"/>
+    <row r="192" s="30" customFormat="1" ht="12.75"/>
+    <row r="193" s="30" customFormat="1" ht="12.75"/>
+    <row r="194" s="30" customFormat="1" ht="12.75"/>
+    <row r="195" s="30" customFormat="1" ht="12.75"/>
+    <row r="196" s="30" customFormat="1" ht="12.75"/>
+    <row r="197" s="30" customFormat="1" ht="12.75"/>
+    <row r="198" s="30" customFormat="1" ht="12.75"/>
+    <row r="199" s="30" customFormat="1" ht="12.75"/>
+    <row r="200" s="30" customFormat="1" ht="12.75"/>
+    <row r="201" s="30" customFormat="1" ht="12.75"/>
+    <row r="202" s="30" customFormat="1" ht="12.75"/>
+    <row r="203" s="30" customFormat="1" ht="12.75"/>
+    <row r="204" s="30" customFormat="1" ht="12.75"/>
+    <row r="205" s="30" customFormat="1" ht="12.75"/>
+    <row r="206" s="30" customFormat="1" ht="12.75"/>
+    <row r="207" s="30" customFormat="1" ht="12.75"/>
+    <row r="208" s="30" customFormat="1" ht="12.75"/>
+    <row r="209" s="30" customFormat="1" ht="12.75"/>
+    <row r="210" s="30" customFormat="1" ht="12.75"/>
+    <row r="211" s="30" customFormat="1" ht="12.75"/>
+    <row r="212" s="30" customFormat="1" ht="12.75"/>
+    <row r="213" s="30" customFormat="1" ht="12.75"/>
+    <row r="214" s="30" customFormat="1" ht="12.75"/>
+    <row r="215" s="30" customFormat="1" ht="12.75"/>
+    <row r="216" s="30" customFormat="1" ht="12.75"/>
+    <row r="217" s="30" customFormat="1" ht="12.75"/>
+    <row r="218" s="30" customFormat="1" ht="12.75"/>
+    <row r="219" s="30" customFormat="1" ht="12.75"/>
+    <row r="220" s="30" customFormat="1" ht="12.75"/>
+    <row r="221" s="30" customFormat="1" ht="12.75"/>
+    <row r="222" s="30" customFormat="1" ht="12.75"/>
+    <row r="223" s="30" customFormat="1" ht="12.75"/>
+    <row r="224" s="30" customFormat="1" ht="12.75"/>
+    <row r="225" s="30" customFormat="1" ht="12.75"/>
+    <row r="226" s="30" customFormat="1" ht="12.75"/>
+    <row r="227" s="30" customFormat="1" ht="12.75"/>
+    <row r="228" s="30" customFormat="1" ht="12.75"/>
+    <row r="229" s="30" customFormat="1" ht="12.75"/>
+    <row r="230" s="30" customFormat="1" ht="12.75"/>
+    <row r="231" s="30" customFormat="1" ht="12.75"/>
+    <row r="232" s="30" customFormat="1" ht="12.75"/>
+    <row r="233" s="30" customFormat="1" ht="12.75"/>
+    <row r="234" s="30" customFormat="1" ht="12.75"/>
+    <row r="235" s="30" customFormat="1" ht="12.75"/>
+    <row r="236" s="30" customFormat="1" ht="12.75"/>
+    <row r="237" s="30" customFormat="1" ht="12.75"/>
+    <row r="238" s="30" customFormat="1" ht="12.75"/>
+    <row r="239" s="30" customFormat="1" ht="12.75"/>
+    <row r="240" s="30" customFormat="1" ht="12.75"/>
+    <row r="241" s="30" customFormat="1" ht="12.75"/>
+    <row r="242" s="30" customFormat="1" ht="12.75"/>
+    <row r="243" s="30" customFormat="1" ht="12.75"/>
+    <row r="244" s="30" customFormat="1" ht="12.75"/>
+    <row r="245" s="30" customFormat="1" ht="12.75"/>
+    <row r="246" s="30" customFormat="1" ht="12.75"/>
+    <row r="247" s="30" customFormat="1" ht="12.75"/>
+    <row r="248" s="30" customFormat="1" ht="12.75"/>
+    <row r="249" s="30" customFormat="1" ht="12.75"/>
+    <row r="250" s="30" customFormat="1" ht="12.75"/>
+    <row r="251" s="30" customFormat="1" ht="12.75"/>
+    <row r="252" s="30" customFormat="1" ht="12.75"/>
+    <row r="253" s="30" customFormat="1" ht="12.75"/>
+    <row r="254" s="30" customFormat="1" ht="12.75"/>
+    <row r="255" s="30" customFormat="1" ht="12.75"/>
+    <row r="256" s="30" customFormat="1" ht="12.75"/>
+    <row r="257" s="30" customFormat="1" ht="12.75"/>
+    <row r="258" s="30" customFormat="1" ht="12.75"/>
+    <row r="259" s="30" customFormat="1" ht="12.75"/>
+    <row r="260" s="30" customFormat="1" ht="12.75"/>
+    <row r="261" s="30" customFormat="1" ht="12.75"/>
+    <row r="262" s="30" customFormat="1" ht="12.75"/>
+    <row r="263" s="30" customFormat="1" ht="12.75"/>
+    <row r="264" s="30" customFormat="1" ht="12.75"/>
+    <row r="265" s="30" customFormat="1" ht="12.75"/>
+    <row r="266" s="30" customFormat="1" ht="12.75"/>
+    <row r="267" s="30" customFormat="1" ht="12.75"/>
+    <row r="268" s="30" customFormat="1" ht="12.75"/>
+    <row r="269" s="30" customFormat="1" ht="12.75"/>
+    <row r="270" s="30" customFormat="1" ht="12.75"/>
+    <row r="271" s="30" customFormat="1" ht="12.75"/>
+    <row r="272" s="30" customFormat="1" ht="12.75"/>
+    <row r="273" s="30" customFormat="1" ht="12.75"/>
+    <row r="274" s="30" customFormat="1" ht="12.75"/>
+    <row r="275" s="30" customFormat="1" ht="12.75"/>
+    <row r="276" s="30" customFormat="1" ht="12.75"/>
+    <row r="277" s="30" customFormat="1" ht="12.75"/>
+    <row r="278" s="30" customFormat="1" ht="12.75"/>
+    <row r="279" s="30" customFormat="1" ht="12.75"/>
+    <row r="280" s="30" customFormat="1" ht="12.75"/>
+    <row r="281" s="30" customFormat="1" ht="12.75"/>
+    <row r="282" s="30" customFormat="1" ht="12.75"/>
+    <row r="283" s="30" customFormat="1" ht="12.75"/>
+    <row r="284" s="30" customFormat="1" ht="12.75"/>
+    <row r="285" s="30" customFormat="1" ht="12.75"/>
+    <row r="286" s="30" customFormat="1" ht="12.75"/>
+    <row r="287" s="30" customFormat="1" ht="12.75"/>
+    <row r="288" s="30" customFormat="1" ht="12.75"/>
+    <row r="289" s="30" customFormat="1" ht="12.75"/>
+    <row r="290" s="30" customFormat="1" ht="12.75"/>
+    <row r="291" s="30" customFormat="1" ht="12.75"/>
+    <row r="292" s="30" customFormat="1" ht="12.75"/>
+    <row r="293" s="30" customFormat="1" ht="12.75"/>
+    <row r="294" s="30" customFormat="1" ht="12.75"/>
+    <row r="295" s="30" customFormat="1" ht="12.75"/>
+    <row r="296" s="30" customFormat="1" ht="12.75"/>
+    <row r="297" s="30" customFormat="1" ht="12.75"/>
+    <row r="298" s="30" customFormat="1" ht="12.75"/>
+    <row r="299" s="30" customFormat="1" ht="12.75"/>
+    <row r="300" s="30" customFormat="1" ht="12.75"/>
+    <row r="301" s="30" customFormat="1" ht="12.75"/>
+    <row r="302" s="30" customFormat="1" ht="12.75"/>
+    <row r="303" s="30" customFormat="1" ht="12.75"/>
+    <row r="304" s="30" customFormat="1" ht="12.75"/>
+    <row r="305" s="30" customFormat="1" ht="12.75"/>
+    <row r="306" s="30" customFormat="1" ht="12.75"/>
+    <row r="307" s="30" customFormat="1" ht="12.75"/>
+    <row r="308" s="30" customFormat="1" ht="12.75"/>
+    <row r="309" s="30" customFormat="1" ht="12.75"/>
+    <row r="310" s="30" customFormat="1" ht="12.75"/>
+    <row r="311" s="30" customFormat="1" ht="12.75"/>
+    <row r="312" s="30" customFormat="1" ht="12.75"/>
+    <row r="313" s="30" customFormat="1" ht="12.75"/>
+    <row r="314" s="30" customFormat="1" ht="12.75"/>
+    <row r="315" s="30" customFormat="1" ht="12.75"/>
+    <row r="316" s="30" customFormat="1" ht="12.75"/>
+    <row r="317" s="30" customFormat="1" ht="12.75"/>
+    <row r="318" s="30" customFormat="1" ht="12.75"/>
+    <row r="319" s="30" customFormat="1" ht="12.75"/>
+    <row r="320" s="30" customFormat="1" ht="12.75"/>
+    <row r="321" s="30" customFormat="1" ht="12.75"/>
+    <row r="322" s="30" customFormat="1" ht="12.75"/>
+    <row r="323" s="30" customFormat="1" ht="12.75"/>
+    <row r="324" s="30" customFormat="1" ht="12.75"/>
+    <row r="325" s="30" customFormat="1" ht="12.75"/>
+    <row r="326" s="30" customFormat="1" ht="12.75"/>
+    <row r="327" s="30" customFormat="1" ht="12.75"/>
+    <row r="328" s="30" customFormat="1" ht="12.75"/>
+    <row r="329" s="30" customFormat="1" ht="12.75"/>
+    <row r="330" s="30" customFormat="1" ht="12.75"/>
+    <row r="331" s="30" customFormat="1" ht="12.75"/>
+    <row r="332" s="30" customFormat="1" ht="12.75"/>
+    <row r="333" s="30" customFormat="1" ht="12.75"/>
+    <row r="334" s="30" customFormat="1" ht="12.75"/>
+    <row r="335" s="30" customFormat="1" ht="12.75"/>
+    <row r="336" s="30" customFormat="1" ht="12.75"/>
+    <row r="337" s="30" customFormat="1" ht="12.75"/>
+    <row r="338" s="30" customFormat="1" ht="12.75"/>
+    <row r="339" s="30" customFormat="1" ht="12.75"/>
+    <row r="340" s="30" customFormat="1" ht="12.75"/>
+    <row r="341" s="30" customFormat="1" ht="12.75"/>
+    <row r="342" s="30" customFormat="1" ht="12.75"/>
+    <row r="343" s="30" customFormat="1" ht="12.75"/>
+    <row r="344" s="30" customFormat="1" ht="12.75"/>
+    <row r="345" s="30" customFormat="1" ht="12.75"/>
+    <row r="346" s="30" customFormat="1" ht="12.75"/>
+    <row r="347" s="30" customFormat="1" ht="12.75"/>
+    <row r="348" s="30" customFormat="1" ht="12.75"/>
+    <row r="349" s="30" customFormat="1" ht="12.75"/>
+    <row r="350" s="30" customFormat="1" ht="12.75"/>
+    <row r="351" s="30" customFormat="1" ht="12.75"/>
+    <row r="352" s="30" customFormat="1" ht="12.75"/>
+    <row r="353" s="30" customFormat="1" ht="12.75"/>
+    <row r="354" s="30" customFormat="1" ht="12.75"/>
+    <row r="355" s="30" customFormat="1" ht="12.75"/>
+    <row r="356" s="30" customFormat="1" ht="12.75"/>
+    <row r="357" s="30" customFormat="1" ht="12.75"/>
+    <row r="358" s="30" customFormat="1" ht="12.75"/>
+    <row r="359" s="30" customFormat="1" ht="12.75"/>
+    <row r="360" s="30" customFormat="1" ht="12.75"/>
+    <row r="361" s="30" customFormat="1" ht="12.75"/>
+    <row r="362" s="30" customFormat="1" ht="12.75"/>
+    <row r="363" s="30" customFormat="1" ht="12.75"/>
+    <row r="364" s="30" customFormat="1" ht="12.75"/>
+    <row r="365" s="30" customFormat="1" ht="12.75"/>
+    <row r="366" s="30" customFormat="1" ht="12.75"/>
+    <row r="367" s="30" customFormat="1" ht="12.75"/>
+    <row r="368" s="30" customFormat="1" ht="12.75"/>
+    <row r="369" s="30" customFormat="1" ht="12.75"/>
+    <row r="370" s="30" customFormat="1" ht="12.75"/>
+    <row r="371" s="30" customFormat="1" ht="12.75"/>
+    <row r="372" s="30" customFormat="1" ht="12.75"/>
+    <row r="373" s="30" customFormat="1" ht="12.75"/>
+    <row r="374" s="30" customFormat="1" ht="12.75"/>
+    <row r="375" s="30" customFormat="1" ht="12.75"/>
+    <row r="376" s="30" customFormat="1" ht="12.75"/>
+    <row r="377" s="30" customFormat="1" ht="12.75"/>
+    <row r="378" s="30" customFormat="1" ht="12.75"/>
+    <row r="379" s="30" customFormat="1" ht="12.75"/>
+    <row r="380" s="30" customFormat="1" ht="12.75"/>
+    <row r="381" s="30" customFormat="1" ht="12.75"/>
+    <row r="382" s="30" customFormat="1" ht="12.75"/>
+    <row r="383" s="30" customFormat="1" ht="12.75"/>
+    <row r="384" s="30" customFormat="1" ht="12.75"/>
+    <row r="385" s="30" customFormat="1" ht="12.75"/>
+    <row r="386" s="30" customFormat="1" ht="12.75"/>
+    <row r="387" s="30" customFormat="1" ht="12.75"/>
+    <row r="388" s="30" customFormat="1" ht="12.75"/>
+    <row r="389" s="30" customFormat="1" ht="12.75"/>
+    <row r="390" s="30" customFormat="1" ht="12.75"/>
+    <row r="391" s="30" customFormat="1" ht="12.75"/>
+    <row r="392" s="30" customFormat="1" ht="12.75"/>
+    <row r="393" s="30" customFormat="1" ht="12.75"/>
+    <row r="394" s="30" customFormat="1" ht="12.75"/>
+    <row r="395" s="30" customFormat="1" ht="12.75"/>
+    <row r="396" s="30" customFormat="1" ht="12.75"/>
+    <row r="397" s="30" customFormat="1" ht="12.75"/>
+    <row r="398" s="30" customFormat="1" ht="12.75"/>
+    <row r="399" s="30" customFormat="1" ht="12.75"/>
+    <row r="400" s="30" customFormat="1" ht="12.75"/>
+    <row r="401" s="30" customFormat="1" ht="12.75"/>
+    <row r="402" s="30" customFormat="1" ht="12.75"/>
+    <row r="403" s="30" customFormat="1" ht="12.75"/>
+    <row r="404" s="30" customFormat="1" ht="12.75"/>
+    <row r="405" s="30" customFormat="1" ht="12.75"/>
+    <row r="406" s="30" customFormat="1" ht="12.75"/>
+    <row r="407" s="30" customFormat="1" ht="12.75"/>
+    <row r="408" s="30" customFormat="1" ht="12.75"/>
+    <row r="409" s="30" customFormat="1" ht="12.75"/>
+    <row r="410" s="30" customFormat="1" ht="12.75"/>
+    <row r="411" s="30" customFormat="1" ht="12.75"/>
+    <row r="412" s="30" customFormat="1" ht="12.75"/>
+    <row r="413" s="30" customFormat="1" ht="12.75"/>
+    <row r="414" s="30" customFormat="1" ht="12.75"/>
+    <row r="415" s="30" customFormat="1" ht="12.75"/>
+    <row r="416" s="30" customFormat="1" ht="12.75"/>
+    <row r="417" s="30" customFormat="1" ht="12.75"/>
+    <row r="418" s="30" customFormat="1" ht="12.75"/>
+    <row r="419" s="30" customFormat="1" ht="12.75"/>
+    <row r="420" s="30" customFormat="1" ht="12.75"/>
+    <row r="421" s="30" customFormat="1" ht="12.75"/>
+    <row r="422" s="30" customFormat="1" ht="12.75"/>
+    <row r="423" s="30" customFormat="1" ht="12.75"/>
+    <row r="424" s="30" customFormat="1" ht="12.75"/>
+    <row r="425" s="30" customFormat="1" ht="12.75"/>
+    <row r="426" s="30" customFormat="1" ht="12.75"/>
+    <row r="427" s="30" customFormat="1" ht="12.75"/>
+    <row r="428" s="30" customFormat="1" ht="12.75"/>
+    <row r="429" s="30" customFormat="1" ht="12.75"/>
+    <row r="430" s="30" customFormat="1" ht="12.75"/>
+    <row r="431" s="30" customFormat="1" ht="12.75"/>
+    <row r="432" s="30" customFormat="1" ht="12.75"/>
+    <row r="433" s="30" customFormat="1" ht="12.75"/>
+    <row r="434" s="30" customFormat="1" ht="12.75"/>
+    <row r="435" s="30" customFormat="1" ht="12.75"/>
+    <row r="436" s="30" customFormat="1" ht="12.75"/>
+    <row r="437" s="30" customFormat="1" ht="12.75"/>
+    <row r="438" s="30" customFormat="1" ht="12.75"/>
+    <row r="439" s="30" customFormat="1" ht="12.75"/>
+    <row r="440" s="30" customFormat="1" ht="12.75"/>
+    <row r="441" s="30" customFormat="1" ht="12.75"/>
+    <row r="442" s="30" customFormat="1" ht="12.75"/>
+    <row r="443" s="30" customFormat="1" ht="12.75"/>
+    <row r="444" s="30" customFormat="1" ht="12.75"/>
+    <row r="445" s="30" customFormat="1" ht="12.75"/>
+    <row r="446" s="30" customFormat="1" ht="12.75"/>
+    <row r="447" s="30" customFormat="1" ht="12.75"/>
+    <row r="448" s="30" customFormat="1" ht="12.75"/>
+    <row r="449" s="30" customFormat="1" ht="12.75"/>
+    <row r="450" s="30" customFormat="1" ht="12.75"/>
+    <row r="451" s="30" customFormat="1" ht="12.75"/>
+    <row r="452" s="30" customFormat="1" ht="12.75"/>
+    <row r="453" s="30" customFormat="1" ht="12.75"/>
+    <row r="454" s="30" customFormat="1" ht="12.75"/>
+    <row r="455" s="30" customFormat="1" ht="12.75"/>
+    <row r="456" s="30" customFormat="1" ht="12.75"/>
+    <row r="457" s="30" customFormat="1" ht="12.75"/>
+    <row r="458" s="30" customFormat="1" ht="12.75"/>
+    <row r="459" s="30" customFormat="1" ht="12.75"/>
+    <row r="460" s="30" customFormat="1" ht="12.75"/>
+    <row r="461" s="30" customFormat="1" ht="12.75"/>
+    <row r="462" s="30" customFormat="1" ht="12.75"/>
+    <row r="463" s="30" customFormat="1" ht="12.75"/>
+    <row r="464" s="30" customFormat="1" ht="12.75"/>
+    <row r="465" s="30" customFormat="1" ht="12.75"/>
+    <row r="466" s="30" customFormat="1" ht="12.75"/>
+    <row r="467" s="30" customFormat="1" ht="12.75"/>
+    <row r="468" s="30" customFormat="1" ht="12.75"/>
+    <row r="469" s="30" customFormat="1" ht="12.75"/>
+    <row r="470" s="30" customFormat="1" ht="12.75"/>
+    <row r="471" s="30" customFormat="1" ht="12.75"/>
+    <row r="472" s="30" customFormat="1" ht="12.75"/>
+    <row r="473" s="30" customFormat="1" ht="12.75"/>
+    <row r="474" s="30" customFormat="1" ht="12.75"/>
+    <row r="475" s="30" customFormat="1" ht="12.75"/>
+    <row r="476" s="30" customFormat="1" ht="12.75"/>
+    <row r="477" s="30" customFormat="1" ht="12.75"/>
+    <row r="478" s="30" customFormat="1" ht="12.75"/>
+    <row r="479" s="30" customFormat="1" ht="12.75"/>
+    <row r="480" s="30" customFormat="1" ht="12.75"/>
+    <row r="481" s="30" customFormat="1" ht="12.75"/>
+    <row r="482" s="30" customFormat="1" ht="12.75"/>
+    <row r="483" s="30" customFormat="1" ht="12.75"/>
+    <row r="484" s="30" customFormat="1" ht="12.75"/>
+    <row r="485" s="30" customFormat="1" ht="12.75"/>
+    <row r="486" s="30" customFormat="1" ht="12.75"/>
+    <row r="487" s="30" customFormat="1" ht="12.75"/>
+    <row r="488" s="30" customFormat="1" ht="12.75"/>
+    <row r="489" s="30" customFormat="1" ht="12.75"/>
+    <row r="490" s="30" customFormat="1" ht="12.75"/>
+    <row r="491" s="30" customFormat="1" ht="12.75"/>
+    <row r="492" s="30" customFormat="1" ht="12.75"/>
+    <row r="493" s="30" customFormat="1" ht="12.75"/>
+    <row r="494" s="30" customFormat="1" ht="12.75"/>
+    <row r="495" s="30" customFormat="1" ht="12.75"/>
+    <row r="496" s="30" customFormat="1" ht="12.75"/>
+    <row r="497" s="30" customFormat="1" ht="12.75"/>
+    <row r="498" s="30" customFormat="1" ht="12.75"/>
+    <row r="499" s="30" customFormat="1" ht="12.75"/>
+    <row r="500" s="30" customFormat="1" ht="12.75"/>
+    <row r="501" s="30" customFormat="1" ht="12.75"/>
+    <row r="502" s="30" customFormat="1" ht="12.75"/>
+    <row r="503" s="30" customFormat="1" ht="12.75"/>
+    <row r="504" s="30" customFormat="1" ht="12.75"/>
+    <row r="505" s="30" customFormat="1" ht="12.75"/>
+    <row r="506" s="30" customFormat="1" ht="12.75"/>
+    <row r="507" s="30" customFormat="1" ht="12.75"/>
+    <row r="508" s="30" customFormat="1" ht="12.75"/>
+    <row r="509" s="30" customFormat="1" ht="12.75"/>
+    <row r="510" s="30" customFormat="1" ht="12.75"/>
+    <row r="511" s="30" customFormat="1" ht="12.75"/>
+    <row r="512" s="30" customFormat="1" ht="12.75"/>
+    <row r="513" s="30" customFormat="1" ht="12.75"/>
+    <row r="514" s="30" customFormat="1" ht="12.75"/>
+    <row r="515" s="30" customFormat="1" ht="12.75"/>
+    <row r="516" s="30" customFormat="1" ht="12.75"/>
+    <row r="517" s="30" customFormat="1" ht="12.75"/>
+    <row r="518" s="30" customFormat="1" ht="12.75"/>
+    <row r="519" s="30" customFormat="1" ht="12.75"/>
+    <row r="520" s="30" customFormat="1" ht="12.75"/>
+    <row r="521" s="30" customFormat="1" ht="12.75"/>
+    <row r="522" s="30" customFormat="1" ht="12.75"/>
+    <row r="523" s="30" customFormat="1" ht="12.75"/>
+    <row r="524" s="30" customFormat="1" ht="12.75"/>
+    <row r="525" s="30" customFormat="1" ht="12.75"/>
+    <row r="526" s="30" customFormat="1" ht="12.75"/>
+    <row r="527" s="30" customFormat="1" ht="12.75"/>
+    <row r="528" s="30" customFormat="1" ht="12.75"/>
+    <row r="529" s="30" customFormat="1" ht="12.75"/>
+    <row r="530" s="30" customFormat="1" ht="12.75"/>
+    <row r="531" s="30" customFormat="1" ht="12.75"/>
+    <row r="532" s="30" customFormat="1" ht="12.75"/>
+    <row r="533" s="30" customFormat="1" ht="12.75"/>
+    <row r="534" s="30" customFormat="1" ht="12.75"/>
+    <row r="535" s="30" customFormat="1" ht="12.75"/>
+    <row r="536" s="30" customFormat="1" ht="12.75"/>
+    <row r="537" s="30" customFormat="1" ht="12.75"/>
+    <row r="538" s="30" customFormat="1" ht="12.75"/>
+    <row r="539" s="30" customFormat="1" ht="12.75"/>
+    <row r="540" s="30" customFormat="1" ht="12.75"/>
+    <row r="541" s="30" customFormat="1" ht="12.75"/>
+    <row r="542" s="30" customFormat="1" ht="12.75"/>
+    <row r="543" s="30" customFormat="1" ht="12.75"/>
+    <row r="544" s="30" customFormat="1" ht="12.75"/>
+    <row r="545" s="30" customFormat="1" ht="12.75"/>
+    <row r="546" s="30" customFormat="1" ht="12.75"/>
+    <row r="547" s="30" customFormat="1" ht="12.75"/>
+    <row r="548" s="30" customFormat="1" ht="12.75"/>
+    <row r="549" s="30" customFormat="1" ht="12.75"/>
+    <row r="550" s="30" customFormat="1" ht="12.75"/>
+    <row r="551" s="30" customFormat="1" ht="12.75"/>
+    <row r="552" s="30" customFormat="1" ht="12.75"/>
+    <row r="553" s="30" customFormat="1" ht="12.75"/>
+    <row r="554" s="30" customFormat="1" ht="12.75"/>
+    <row r="555" s="30" customFormat="1" ht="12.75"/>
+    <row r="556" s="30" customFormat="1" ht="12.75"/>
+    <row r="557" s="30" customFormat="1" ht="12.75"/>
+    <row r="558" s="30" customFormat="1" ht="12.75"/>
+    <row r="559" s="30" customFormat="1" ht="12.75"/>
+    <row r="560" s="30" customFormat="1" ht="12.75"/>
+    <row r="561" s="30" customFormat="1" ht="12.75"/>
+    <row r="562" s="30" customFormat="1" ht="12.75"/>
+    <row r="563" s="30" customFormat="1" ht="12.75"/>
+    <row r="564" s="30" customFormat="1" ht="12.75"/>
+    <row r="565" s="30" customFormat="1" ht="12.75"/>
+    <row r="566" s="30" customFormat="1" ht="12.75"/>
+    <row r="567" s="30" customFormat="1" ht="12.75"/>
+    <row r="568" s="30" customFormat="1" ht="12.75"/>
+    <row r="569" s="30" customFormat="1" ht="12.75"/>
+    <row r="570" s="30" customFormat="1" ht="12.75"/>
+    <row r="571" s="30" customFormat="1" ht="12.75"/>
+    <row r="572" s="30" customFormat="1" ht="12.75"/>
+    <row r="573" s="30" customFormat="1" ht="12.75"/>
+    <row r="574" s="30" customFormat="1" ht="12.75"/>
+    <row r="575" s="30" customFormat="1" ht="12.75"/>
+    <row r="576" s="30" customFormat="1" ht="12.75"/>
+    <row r="577" s="30" customFormat="1" ht="12.75"/>
+    <row r="578" s="30" customFormat="1" ht="12.75"/>
+    <row r="579" s="30" customFormat="1" ht="12.75"/>
+    <row r="580" s="30" customFormat="1" ht="12.75"/>
+    <row r="581" s="30" customFormat="1" ht="12.75"/>
+    <row r="582" s="30" customFormat="1" ht="12.75"/>
+    <row r="583" s="30" customFormat="1" ht="12.75"/>
+    <row r="584" s="30" customFormat="1" ht="12.75"/>
+    <row r="585" s="30" customFormat="1" ht="12.75"/>
+    <row r="586" s="30" customFormat="1" ht="12.75"/>
+    <row r="587" s="30" customFormat="1" ht="12.75"/>
+    <row r="588" s="30" customFormat="1" ht="12.75"/>
+    <row r="589" s="30" customFormat="1" ht="12.75"/>
+    <row r="590" s="30" customFormat="1" ht="12.75"/>
+    <row r="591" s="30" customFormat="1" ht="12.75"/>
+    <row r="592" s="30" customFormat="1" ht="12.75"/>
+    <row r="593" s="30" customFormat="1" ht="12.75"/>
+    <row r="594" s="30" customFormat="1" ht="12.75"/>
+    <row r="595" s="30" customFormat="1" ht="12.75"/>
+    <row r="596" s="30" customFormat="1" ht="12.75"/>
+    <row r="597" s="30" customFormat="1" ht="12.75"/>
+    <row r="598" s="30" customFormat="1" ht="12.75"/>
+    <row r="599" s="30" customFormat="1" ht="12.75"/>
+    <row r="600" s="30" customFormat="1" ht="12.75"/>
+    <row r="601" s="30" customFormat="1" ht="12.75"/>
+    <row r="602" s="30" customFormat="1" ht="12.75"/>
+    <row r="603" s="30" customFormat="1" ht="12.75"/>
+    <row r="604" s="30" customFormat="1" ht="12.75"/>
+    <row r="605" s="30" customFormat="1" ht="12.75"/>
+    <row r="606" s="30" customFormat="1" ht="12.75"/>
+    <row r="607" s="30" customFormat="1" ht="12.75"/>
+    <row r="608" s="30" customFormat="1" ht="12.75"/>
+    <row r="609" s="30" customFormat="1" ht="12.75"/>
+    <row r="610" s="30" customFormat="1" ht="12.75"/>
+    <row r="611" s="30" customFormat="1" ht="12.75"/>
+    <row r="612" s="30" customFormat="1" ht="12.75"/>
+    <row r="613" s="30" customFormat="1" ht="12.75"/>
+    <row r="614" s="30" customFormat="1" ht="12.75"/>
+    <row r="615" s="30" customFormat="1" ht="12.75"/>
+    <row r="616" s="30" customFormat="1" ht="12.75"/>
+    <row r="617" s="30" customFormat="1" ht="12.75"/>
+    <row r="618" s="30" customFormat="1" ht="12.75"/>
+    <row r="619" s="30" customFormat="1" ht="12.75"/>
+    <row r="620" s="30" customFormat="1" ht="12.75"/>
+    <row r="621" s="30" customFormat="1" ht="12.75"/>
+    <row r="622" s="30" customFormat="1" ht="12.75"/>
+    <row r="623" s="30" customFormat="1" ht="12.75"/>
+    <row r="624" s="30" customFormat="1" ht="12.75"/>
+    <row r="625" s="30" customFormat="1" ht="12.75"/>
+    <row r="626" s="30" customFormat="1" ht="12.75"/>
+    <row r="627" s="30" customFormat="1" ht="12.75"/>
+    <row r="628" s="30" customFormat="1" ht="12.75"/>
+    <row r="629" s="30" customFormat="1" ht="12.75"/>
+    <row r="630" s="30" customFormat="1" ht="12.75"/>
+    <row r="631" s="30" customFormat="1" ht="12.75"/>
+    <row r="632" s="30" customFormat="1" ht="12.75"/>
+    <row r="633" s="30" customFormat="1" ht="12.75"/>
+    <row r="634" s="30" customFormat="1" ht="12.75"/>
+    <row r="635" s="30" customFormat="1" ht="12.75"/>
+    <row r="636" s="30" customFormat="1" ht="12.75"/>
+    <row r="637" s="30" customFormat="1" ht="12.75"/>
+    <row r="638" s="30" customFormat="1" ht="12.75"/>
+    <row r="639" s="30" customFormat="1" ht="12.75"/>
+    <row r="640" s="30" customFormat="1" ht="12.75"/>
+    <row r="641" s="30" customFormat="1" ht="12.75"/>
+    <row r="642" s="30" customFormat="1" ht="12.75"/>
+    <row r="643" s="30" customFormat="1" ht="12.75"/>
+    <row r="644" s="30" customFormat="1" ht="12.75"/>
+    <row r="645" s="30" customFormat="1" ht="12.75"/>
+    <row r="646" s="30" customFormat="1" ht="12.75"/>
+    <row r="647" s="30" customFormat="1" ht="12.75"/>
+    <row r="648" s="30" customFormat="1" ht="12.75"/>
+    <row r="649" s="30" customFormat="1" ht="12.75"/>
+    <row r="650" s="30" customFormat="1" ht="12.75"/>
+    <row r="651" s="30" customFormat="1" ht="12.75"/>
+    <row r="652" s="30" customFormat="1" ht="12.75"/>
+    <row r="653" s="30" customFormat="1" ht="12.75"/>
+    <row r="654" s="30" customFormat="1" ht="12.75"/>
+    <row r="655" s="30" customFormat="1" ht="12.75"/>
+    <row r="656" s="30" customFormat="1" ht="12.75"/>
+    <row r="657" s="30" customFormat="1" ht="12.75"/>
+    <row r="658" s="30" customFormat="1" ht="12.75"/>
+    <row r="659" s="30" customFormat="1" ht="12.75"/>
+    <row r="660" s="30" customFormat="1" ht="12.75"/>
+    <row r="661" s="30" customFormat="1" ht="12.75"/>
+    <row r="662" s="30" customFormat="1" ht="12.75"/>
+    <row r="663" s="30" customFormat="1" ht="12.75"/>
+    <row r="664" s="30" customFormat="1" ht="12.75"/>
+    <row r="665" s="30" customFormat="1" ht="12.75"/>
+    <row r="666" s="30" customFormat="1" ht="12.75"/>
+    <row r="667" s="30" customFormat="1" ht="12.75"/>
+    <row r="668" s="30" customFormat="1" ht="12.75"/>
+    <row r="669" s="30" customFormat="1" ht="12.75"/>
+    <row r="670" s="30" customFormat="1" ht="12.75"/>
+    <row r="671" s="30" customFormat="1" ht="12.75"/>
+    <row r="672" s="30" customFormat="1" ht="12.75"/>
+    <row r="673" s="30" customFormat="1" ht="12.75"/>
+    <row r="674" s="30" customFormat="1" ht="12.75"/>
+    <row r="675" s="30" customFormat="1" ht="12.75"/>
+    <row r="676" s="30" customFormat="1" ht="12.75"/>
+    <row r="677" s="30" customFormat="1" ht="12.75"/>
+    <row r="678" s="30" customFormat="1" ht="12.75"/>
+    <row r="679" s="30" customFormat="1" ht="12.75"/>
+    <row r="680" s="30" customFormat="1" ht="12.75"/>
+    <row r="681" s="30" customFormat="1" ht="12.75"/>
+    <row r="682" s="30" customFormat="1" ht="12.75"/>
+    <row r="683" s="30" customFormat="1" ht="12.75"/>
+    <row r="684" s="30" customFormat="1" ht="12.75"/>
+    <row r="685" s="30" customFormat="1" ht="12.75"/>
+    <row r="686" s="30" customFormat="1" ht="12.75"/>
+    <row r="687" s="30" customFormat="1" ht="12.75"/>
+    <row r="688" s="30" customFormat="1" ht="12.75"/>
+    <row r="689" s="30" customFormat="1" ht="12.75"/>
+    <row r="690" s="30" customFormat="1" ht="12.75"/>
+    <row r="691" s="30" customFormat="1" ht="12.75"/>
+    <row r="692" s="30" customFormat="1" ht="12.75"/>
+    <row r="693" s="30" customFormat="1" ht="12.75"/>
+    <row r="694" s="30" customFormat="1" ht="12.75"/>
+    <row r="695" s="30" customFormat="1" ht="12.75"/>
+    <row r="696" s="30" customFormat="1" ht="12.75"/>
+    <row r="697" s="30" customFormat="1" ht="12.75"/>
+    <row r="698" s="30" customFormat="1" ht="12.75"/>
+    <row r="699" s="30" customFormat="1" ht="12.75"/>
+    <row r="700" s="30" customFormat="1" ht="12.75"/>
+    <row r="701" s="30" customFormat="1" ht="12.75"/>
+    <row r="702" s="30" customFormat="1" ht="12.75"/>
+    <row r="703" s="30" customFormat="1" ht="12.75"/>
+    <row r="704" s="30" customFormat="1" ht="12.75"/>
+    <row r="705" s="30" customFormat="1" ht="12.75"/>
+    <row r="706" s="30" customFormat="1" ht="12.75"/>
+    <row r="707" s="30" customFormat="1" ht="12.75"/>
+    <row r="708" s="30" customFormat="1" ht="12.75"/>
+    <row r="709" s="30" customFormat="1" ht="12.75"/>
+    <row r="710" s="30" customFormat="1" ht="12.75"/>
+    <row r="711" s="30" customFormat="1" ht="12.75"/>
+    <row r="712" s="30" customFormat="1" ht="12.75"/>
+    <row r="713" s="30" customFormat="1" ht="12.75"/>
+    <row r="714" s="30" customFormat="1" ht="12.75"/>
+    <row r="715" s="30" customFormat="1" ht="12.75"/>
+    <row r="716" s="30" customFormat="1" ht="12.75"/>
+    <row r="717" s="30" customFormat="1" ht="12.75"/>
+    <row r="718" s="30" customFormat="1" ht="12.75"/>
+    <row r="719" s="30" customFormat="1" ht="12.75"/>
+    <row r="720" s="30" customFormat="1" ht="12.75"/>
+    <row r="721" s="30" customFormat="1" ht="12.75"/>
+    <row r="722" s="30" customFormat="1" ht="12.75"/>
+    <row r="723" s="30" customFormat="1" ht="12.75"/>
+    <row r="724" s="30" customFormat="1" ht="12.75"/>
+    <row r="725" s="30" customFormat="1" ht="12.75"/>
+    <row r="726" s="30" customFormat="1" ht="12.75"/>
+    <row r="727" s="30" customFormat="1" ht="12.75"/>
+    <row r="728" s="30" customFormat="1" ht="12.75"/>
+    <row r="729" s="30" customFormat="1" ht="12.75"/>
+    <row r="730" s="30" customFormat="1" ht="12.75"/>
+    <row r="731" s="30" customFormat="1" ht="12.75"/>
+    <row r="732" s="30" customFormat="1" ht="12.75"/>
+    <row r="733" s="30" customFormat="1" ht="12.75"/>
+    <row r="734" s="30" customFormat="1" ht="12.75"/>
+    <row r="735" s="30" customFormat="1" ht="12.75"/>
+    <row r="736" s="30" customFormat="1" ht="12.75"/>
+    <row r="737" s="30" customFormat="1" ht="12.75"/>
+    <row r="738" s="30" customFormat="1" ht="12.75"/>
+    <row r="739" s="30" customFormat="1" ht="12.75"/>
+    <row r="740" s="30" customFormat="1" ht="12.75"/>
+    <row r="741" s="30" customFormat="1" ht="12.75"/>
+    <row r="742" s="30" customFormat="1" ht="12.75"/>
+    <row r="743" s="30" customFormat="1" ht="12.75"/>
+    <row r="744" s="30" customFormat="1" ht="12.75"/>
+    <row r="745" s="30" customFormat="1" ht="12.75"/>
+    <row r="746" s="30" customFormat="1" ht="12.75"/>
+    <row r="747" s="30" customFormat="1" ht="12.75"/>
+    <row r="748" s="30" customFormat="1" ht="12.75"/>
+    <row r="749" s="30" customFormat="1" ht="12.75"/>
+    <row r="750" s="30" customFormat="1" ht="12.75"/>
+    <row r="751" s="30" customFormat="1" ht="12.75"/>
+    <row r="752" s="30" customFormat="1" ht="12.75"/>
+    <row r="753" s="30" customFormat="1" ht="12.75"/>
+    <row r="754" s="30" customFormat="1" ht="12.75"/>
+    <row r="755" s="30" customFormat="1" ht="12.75"/>
+    <row r="756" s="30" customFormat="1" ht="12.75"/>
+    <row r="757" s="30" customFormat="1" ht="12.75"/>
+    <row r="758" s="30" customFormat="1" ht="12.75"/>
+    <row r="759" s="30" customFormat="1" ht="12.75"/>
+    <row r="760" s="30" customFormat="1" ht="12.75"/>
+    <row r="761" s="30" customFormat="1" ht="12.75"/>
+    <row r="762" s="30" customFormat="1" ht="12.75"/>
+    <row r="763" s="30" customFormat="1" ht="12.75"/>
+    <row r="764" s="30" customFormat="1" ht="12.75"/>
+    <row r="765" s="30" customFormat="1" ht="12.75"/>
+    <row r="766" s="30" customFormat="1" ht="12.75"/>
+    <row r="767" s="30" customFormat="1" ht="12.75"/>
+    <row r="768" s="30" customFormat="1" ht="12.75"/>
+    <row r="769" s="30" customFormat="1" ht="12.75"/>
+    <row r="770" s="30" customFormat="1" ht="12.75"/>
+    <row r="771" s="30" customFormat="1" ht="12.75"/>
+    <row r="772" s="30" customFormat="1" ht="12.75"/>
+    <row r="773" s="30" customFormat="1" ht="12.75"/>
+    <row r="774" s="30" customFormat="1" ht="12.75"/>
+    <row r="775" s="30" customFormat="1" ht="12.75"/>
+    <row r="776" s="30" customFormat="1" ht="12.75"/>
+    <row r="777" s="30" customFormat="1" ht="12.75"/>
+    <row r="778" s="30" customFormat="1" ht="12.75"/>
+    <row r="779" s="30" customFormat="1" ht="12.75"/>
+    <row r="780" s="30" customFormat="1" ht="12.75"/>
+    <row r="781" s="30" customFormat="1" ht="12.75"/>
+    <row r="782" s="30" customFormat="1" ht="12.75"/>
+    <row r="783" s="30" customFormat="1" ht="12.75"/>
+    <row r="784" s="30" customFormat="1" ht="12.75"/>
+    <row r="785" s="30" customFormat="1" ht="12.75"/>
+    <row r="786" s="30" customFormat="1" ht="12.75"/>
+    <row r="787" s="30" customFormat="1" ht="12.75"/>
+    <row r="788" s="30" customFormat="1" ht="12.75"/>
+    <row r="789" s="30" customFormat="1" ht="12.75"/>
+    <row r="790" s="30" customFormat="1" ht="12.75"/>
+    <row r="791" s="30" customFormat="1" ht="12.75"/>
+    <row r="792" s="30" customFormat="1" ht="12.75"/>
+    <row r="793" s="30" customFormat="1" ht="12.75"/>
+    <row r="794" s="30" customFormat="1" ht="12.75"/>
+    <row r="795" s="30" customFormat="1" ht="12.75"/>
+    <row r="796" s="30" customFormat="1" ht="12.75"/>
+    <row r="797" s="30" customFormat="1" ht="12.75"/>
+    <row r="798" s="30" customFormat="1" ht="12.75"/>
+    <row r="799" s="30" customFormat="1" ht="12.75"/>
+    <row r="800" s="30" customFormat="1" ht="12.75"/>
+    <row r="801" s="30" customFormat="1" ht="12.75"/>
+    <row r="802" s="30" customFormat="1" ht="12.75"/>
+    <row r="803" s="30" customFormat="1" ht="12.75"/>
+    <row r="804" s="30" customFormat="1" ht="12.75"/>
+    <row r="805" s="30" customFormat="1" ht="12.75"/>
+    <row r="806" s="30" customFormat="1" ht="12.75"/>
+    <row r="807" s="30" customFormat="1" ht="12.75"/>
+    <row r="808" s="30" customFormat="1" ht="12.75"/>
+    <row r="809" s="30" customFormat="1" ht="12.75"/>
+    <row r="810" s="30" customFormat="1" ht="12.75"/>
+    <row r="811" s="30" customFormat="1" ht="12.75"/>
+    <row r="812" s="30" customFormat="1" ht="12.75"/>
+    <row r="813" s="30" customFormat="1" ht="12.75"/>
+    <row r="814" s="30" customFormat="1" ht="12.75"/>
+    <row r="815" s="30" customFormat="1" ht="12.75"/>
+    <row r="816" s="30" customFormat="1" ht="12.75"/>
+    <row r="817" s="30" customFormat="1" ht="12.75"/>
+    <row r="818" s="30" customFormat="1" ht="12.75"/>
+    <row r="819" s="30" customFormat="1" ht="12.75"/>
+    <row r="820" s="30" customFormat="1" ht="12.75"/>
+    <row r="821" s="30" customFormat="1" ht="12.75"/>
+    <row r="822" s="30" customFormat="1" ht="12.75"/>
+    <row r="823" s="30" customFormat="1" ht="12.75"/>
+    <row r="824" s="30" customFormat="1" ht="12.75"/>
+    <row r="825" s="30" customFormat="1" ht="12.75"/>
+    <row r="826" s="30" customFormat="1" ht="12.75"/>
+    <row r="827" s="30" customFormat="1" ht="12.75"/>
+    <row r="828" s="30" customFormat="1" ht="12.75"/>
+    <row r="829" s="30" customFormat="1" ht="12.75"/>
+    <row r="830" s="30" customFormat="1" ht="12.75"/>
+    <row r="831" s="30" customFormat="1" ht="12.75"/>
+    <row r="832" s="30" customFormat="1" ht="12.75"/>
+    <row r="833" s="30" customFormat="1" ht="12.75"/>
+    <row r="834" s="30" customFormat="1" ht="12.75"/>
+    <row r="835" s="30" customFormat="1" ht="12.75"/>
+    <row r="836" s="30" customFormat="1" ht="12.75"/>
+    <row r="837" s="30" customFormat="1" ht="12.75"/>
+    <row r="838" s="30" customFormat="1" ht="12.75"/>
+    <row r="839" s="30" customFormat="1" ht="12.75"/>
+    <row r="840" s="30" customFormat="1" ht="12.75"/>
+    <row r="841" s="30" customFormat="1" ht="12.75"/>
+    <row r="842" s="30" customFormat="1" ht="12.75"/>
+    <row r="843" s="30" customFormat="1" ht="12.75"/>
+    <row r="844" s="30" customFormat="1" ht="12.75"/>
+    <row r="845" s="30" customFormat="1" ht="12.75"/>
+    <row r="846" s="30" customFormat="1" ht="12.75"/>
+    <row r="847" s="30" customFormat="1" ht="12.75"/>
+    <row r="848" s="30" customFormat="1" ht="12.75"/>
+    <row r="849" s="30" customFormat="1" ht="12.75"/>
+    <row r="850" s="30" customFormat="1" ht="12.75"/>
+    <row r="851" s="30" customFormat="1" ht="12.75"/>
+    <row r="852" s="30" customFormat="1" ht="12.75"/>
+    <row r="853" s="30" customFormat="1" ht="12.75"/>
+    <row r="854" s="30" customFormat="1" ht="12.75"/>
+    <row r="855" s="30" customFormat="1" ht="12.75"/>
+    <row r="856" s="30" customFormat="1" ht="12.75"/>
+    <row r="857" s="30" customFormat="1" ht="12.75"/>
+    <row r="858" s="30" customFormat="1" ht="12.75"/>
+    <row r="859" s="30" customFormat="1" ht="12.75"/>
+    <row r="860" s="30" customFormat="1" ht="12.75"/>
+    <row r="861" s="30" customFormat="1" ht="12.75"/>
+    <row r="862" s="30" customFormat="1" ht="12.75"/>
+    <row r="863" s="30" customFormat="1" ht="12.75"/>
+    <row r="864" s="30" customFormat="1" ht="12.75"/>
+    <row r="865" s="30" customFormat="1" ht="12.75"/>
+    <row r="866" s="30" customFormat="1" ht="12.75"/>
+    <row r="867" s="30" customFormat="1" ht="12.75"/>
+    <row r="868" s="30" customFormat="1" ht="12.75"/>
+    <row r="869" s="30" customFormat="1" ht="12.75"/>
+    <row r="870" s="30" customFormat="1" ht="12.75"/>
+    <row r="871" s="30" customFormat="1" ht="12.75"/>
+    <row r="872" s="30" customFormat="1" ht="12.75"/>
+    <row r="873" s="30" customFormat="1" ht="12.75"/>
+    <row r="874" s="30" customFormat="1" ht="12.75"/>
+    <row r="875" s="30" customFormat="1" ht="12.75"/>
+    <row r="876" s="30" customFormat="1" ht="12.75"/>
+    <row r="877" s="30" customFormat="1" ht="12.75"/>
+    <row r="878" s="30" customFormat="1" ht="12.75"/>
+    <row r="879" s="30" customFormat="1" ht="12.75"/>
+    <row r="880" s="30" customFormat="1" ht="12.75"/>
+    <row r="881" s="30" customFormat="1" ht="12.75"/>
+    <row r="882" s="30" customFormat="1" ht="12.75"/>
+    <row r="883" s="30" customFormat="1" ht="12.75"/>
+    <row r="884" s="30" customFormat="1" ht="12.75"/>
+    <row r="885" s="30" customFormat="1" ht="12.75"/>
+    <row r="886" s="30" customFormat="1" ht="12.75"/>
+    <row r="887" s="30" customFormat="1" ht="12.75"/>
+    <row r="888" s="30" customFormat="1" ht="12.75"/>
+    <row r="889" s="30" customFormat="1" ht="12.75"/>
+    <row r="890" s="30" customFormat="1" ht="12.75"/>
+    <row r="891" s="30" customFormat="1" ht="12.75"/>
+    <row r="892" s="30" customFormat="1" ht="12.75"/>
+    <row r="893" s="30" customFormat="1" ht="12.75"/>
+    <row r="894" s="30" customFormat="1" ht="12.75"/>
+    <row r="895" s="30" customFormat="1" ht="12.75"/>
+    <row r="896" s="30" customFormat="1" ht="12.75"/>
+    <row r="897" s="30" customFormat="1" ht="12.75"/>
+    <row r="898" s="30" customFormat="1" ht="12.75"/>
+    <row r="899" s="30" customFormat="1" ht="12.75"/>
+    <row r="900" s="30" customFormat="1" ht="12.75"/>
+    <row r="901" s="30" customFormat="1" ht="12.75"/>
+    <row r="902" s="30" customFormat="1" ht="12.75"/>
+    <row r="903" s="30" customFormat="1" ht="12.75"/>
+    <row r="904" s="30" customFormat="1" ht="12.75"/>
+    <row r="905" s="30" customFormat="1" ht="12.75"/>
+    <row r="906" s="30" customFormat="1" ht="12.75"/>
+    <row r="907" s="30" customFormat="1" ht="12.75"/>
+    <row r="908" s="30" customFormat="1" ht="12.75"/>
+    <row r="909" s="30" customFormat="1" ht="12.75"/>
+    <row r="910" s="30" customFormat="1" ht="12.75"/>
+    <row r="911" s="30" customFormat="1" ht="12.75"/>
+    <row r="912" s="30" customFormat="1" ht="12.75"/>
+    <row r="913" s="30" customFormat="1" ht="12.75"/>
+    <row r="914" s="30" customFormat="1" ht="12.75"/>
+    <row r="915" s="30" customFormat="1" ht="12.75"/>
+    <row r="916" s="30" customFormat="1" ht="12.75"/>
+    <row r="917" s="30" customFormat="1" ht="12.75"/>
+    <row r="918" s="30" customFormat="1" ht="12.75"/>
+    <row r="919" s="30" customFormat="1" ht="12.75"/>
+    <row r="920" s="30" customFormat="1" ht="12.75"/>
+    <row r="921" s="30" customFormat="1" ht="12.75"/>
+    <row r="922" s="30" customFormat="1" ht="12.75"/>
+    <row r="923" s="30" customFormat="1" ht="12.75"/>
+    <row r="924" s="30" customFormat="1" ht="12.75"/>
+    <row r="925" s="30" customFormat="1" ht="12.75"/>
+    <row r="926" s="30" customFormat="1" ht="12.75"/>
+    <row r="927" s="30" customFormat="1" ht="12.75"/>
+    <row r="928" s="30" customFormat="1" ht="12.75"/>
+    <row r="929" s="30" customFormat="1" ht="12.75"/>
+    <row r="930" s="30" customFormat="1" ht="12.75"/>
+    <row r="931" s="30" customFormat="1" ht="12.75"/>
+    <row r="932" s="30" customFormat="1" ht="12.75"/>
+    <row r="933" s="30" customFormat="1" ht="12.75"/>
+    <row r="934" s="30" customFormat="1" ht="12.75"/>
+    <row r="935" s="30" customFormat="1" ht="12.75"/>
+    <row r="936" s="30" customFormat="1" ht="12.75"/>
+    <row r="937" s="30" customFormat="1" ht="12.75"/>
+    <row r="938" s="30" customFormat="1" ht="12.75"/>
+    <row r="939" s="30" customFormat="1" ht="12.75"/>
+    <row r="940" s="30" customFormat="1" ht="12.75"/>
+    <row r="941" s="30" customFormat="1" ht="12.75"/>
+    <row r="942" s="30" customFormat="1" ht="12.75"/>
+    <row r="943" s="30" customFormat="1" ht="12.75"/>
+    <row r="944" s="30" customFormat="1" ht="12.75"/>
+    <row r="945" s="30" customFormat="1" ht="12.75"/>
+    <row r="946" s="30" customFormat="1" ht="12.75"/>
+    <row r="947" s="30" customFormat="1" ht="12.75"/>
+    <row r="948" s="30" customFormat="1" ht="12.75"/>
+    <row r="949" s="30" customFormat="1" ht="12.75"/>
+    <row r="950" s="30" customFormat="1" ht="12.75"/>
+    <row r="951" s="30" customFormat="1" ht="12.75"/>
+    <row r="952" s="30" customFormat="1" ht="12.75"/>
+    <row r="953" s="30" customFormat="1" ht="12.75"/>
+    <row r="954" s="30" customFormat="1" ht="12.75"/>
+    <row r="955" s="30" customFormat="1" ht="12.75"/>
+    <row r="956" s="30" customFormat="1" ht="12.75"/>
+    <row r="957" s="30" customFormat="1" ht="12.75"/>
+    <row r="958" s="30" customFormat="1" ht="12.75"/>
+    <row r="959" s="30" customFormat="1" ht="12.75"/>
+    <row r="960" s="30" customFormat="1" ht="12.75"/>
+    <row r="961" s="30" customFormat="1" ht="12.75"/>
+    <row r="962" s="30" customFormat="1" ht="12.75"/>
+    <row r="963" s="30" customFormat="1" ht="12.75"/>
+    <row r="964" s="30" customFormat="1" ht="12.75"/>
+    <row r="965" s="30" customFormat="1" ht="12.75"/>
+    <row r="966" s="30" customFormat="1" ht="12.75"/>
+    <row r="967" s="30" customFormat="1" ht="12.75"/>
+    <row r="968" s="30" customFormat="1" ht="12.75"/>
+    <row r="969" s="30" customFormat="1" ht="12.75"/>
+    <row r="970" s="30" customFormat="1" ht="12.75"/>
+    <row r="971" s="30" customFormat="1" ht="12.75"/>
+    <row r="972" s="30" customFormat="1" ht="12.75"/>
+    <row r="973" s="30" customFormat="1" ht="12.75"/>
+    <row r="974" s="30" customFormat="1" ht="12.75"/>
+    <row r="975" s="30" customFormat="1" ht="12.75"/>
+    <row r="976" s="30" customFormat="1" ht="12.75"/>
+    <row r="977" s="30" customFormat="1" ht="12.75"/>
+    <row r="978" s="30" customFormat="1" ht="12.75"/>
+    <row r="979" s="30" customFormat="1" ht="12.75"/>
+    <row r="980" s="30" customFormat="1" ht="12.75"/>
+    <row r="981" s="30" customFormat="1" ht="12.75"/>
+    <row r="982" s="30" customFormat="1" ht="12.75"/>
+    <row r="983" s="30" customFormat="1" ht="12.75"/>
+    <row r="984" s="30" customFormat="1" ht="12.75"/>
+    <row r="985" s="30" customFormat="1" ht="12.75"/>
+    <row r="986" s="30" customFormat="1" ht="12.75"/>
+    <row r="987" s="30" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:A3"/>
@@ -12756,13 +12763,13 @@
       <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>985</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>986</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>987</v>
       </c>
       <c r="D2" s="57" t="s">
@@ -12786,36 +12793,36 @@
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="22" t="s">
         <v>991</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="22" t="s">
         <v>992</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="52"/>
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>993</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="22" t="s">
         <v>994</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="52"/>
@@ -12836,13 +12843,13 @@
       <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>997</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>998</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>999</v>
       </c>
       <c r="D6" s="53" t="s">
@@ -12898,16 +12905,16 @@
       <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="30.75" customHeight="1">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="47" t="s">
         <v>1007</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="48" t="s">
         <v>1008</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="48" t="s">
         <v>1009</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="49" t="s">
         <v>1010</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -12924,10 +12931,10 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="12.75">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="11" t="s">
         <v>1013</v>
       </c>
@@ -12942,13 +12949,13 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="12.75">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="38" t="s">
         <v>1015</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="37" t="s">
         <v>1016</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="37" t="s">
         <v>1016</v>
       </c>
       <c r="D11" s="53" t="s">
@@ -12986,13 +12993,13 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="38" t="s">
         <v>1022</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="37" t="s">
         <v>1023</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="37" t="s">
         <v>1024</v>
       </c>
       <c r="D13" s="57" t="s">
@@ -13030,13 +13037,13 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>1030</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="37" t="s">
         <v>1031</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="37" t="s">
         <v>1032</v>
       </c>
       <c r="D15" s="57" t="s">
@@ -13074,13 +13081,13 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="38" t="s">
         <v>1038</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>1039</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="37" t="s">
         <v>1039</v>
       </c>
       <c r="D17" s="53" t="s">
@@ -13127,7 +13134,7 @@
       <c r="C19" s="8" t="s">
         <v>1047</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="27" t="s">
         <v>1048</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -13170,13 +13177,13 @@
       <c r="L20" s="11"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="38" t="s">
         <v>1056</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="37" t="s">
         <v>1057</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="37" t="s">
         <v>1057</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -13199,21 +13206,21 @@
       <c r="A22" s="52"/>
       <c r="B22" s="52"/>
       <c r="C22" s="52"/>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="27" t="s">
         <v>1061</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="22" t="s">
         <v>1062</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="22" t="s">
         <v>1063</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
     </row>
     <row r="23" spans="1:12" ht="41.25">
       <c r="A23" s="11" t="s">
@@ -13249,7 +13256,7 @@
       <c r="C24" s="8" t="s">
         <v>1071</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="27" t="s">
         <v>1072</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -13349,16 +13356,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="49.5" customHeight="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>1075</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>1076</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>1076</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>1077</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -13401,16 +13408,16 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="38" t="s">
         <v>1087</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>1088</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>1089</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="50" t="s">
         <v>1090</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -13473,16 +13480,16 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="34.5" customHeight="1">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>1106</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="37" t="s">
         <v>1107</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="37" t="s">
         <v>1107</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="50" t="s">
         <v>1108</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -13534,7 +13541,7 @@
       <c r="C12" s="8" t="s">
         <v>1120</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="28" t="s">
         <v>1121</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -13723,16 +13730,16 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="47.25" customHeight="1">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="38" t="s">
         <v>1172</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="37" t="s">
         <v>1173</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="37" t="s">
         <v>1174</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="50" t="s">
         <v>1175</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -13767,16 +13774,16 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="27" customHeight="1">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="38" t="s">
         <v>1182</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="37" t="s">
         <v>1183</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="37" t="s">
         <v>1184</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="50" t="s">
         <v>1185</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -13849,7 +13856,7 @@
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13857,7 +13864,7 @@
       <c r="A3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>75</v>
       </c>
     </row>
@@ -13877,8 +13884,8 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13931,7 +13938,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="47.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>88</v>
       </c>
@@ -13951,7 +13958,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="67.5" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>94</v>
       </c>
@@ -13971,7 +13978,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="92.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>97</v>
       </c>
@@ -14007,21 +14014,21 @@
       <c r="E6" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="35" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:6" ht="116.25" customHeight="1">
+      <c r="A7" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="36" t="s">
         <v>106</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -14031,7 +14038,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="116.25" customHeight="1">
       <c r="A8" s="52"/>
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
@@ -14039,11 +14046,11 @@
       <c r="E8" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="35" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="116.25" customHeight="1">
       <c r="A9" s="52"/>
       <c r="B9" s="52"/>
       <c r="C9" s="52"/>
@@ -14051,11 +14058,11 @@
       <c r="E9" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="35" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="94.5" customHeight="1">
       <c r="A10" s="52"/>
       <c r="B10" s="52"/>
       <c r="C10" s="52"/>
@@ -14063,11 +14070,11 @@
       <c r="E10" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="35" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="66.75" customHeight="1">
       <c r="A11" s="52"/>
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
@@ -14075,21 +14082,21 @@
       <c r="E11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="35" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="35" t="s">
+    <row r="12" spans="1:6" ht="116.25" customHeight="1">
+      <c r="A12" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="36" t="s">
         <v>123</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -14099,7 +14106,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="116.25" customHeight="1">
       <c r="A13" s="52"/>
       <c r="B13" s="52"/>
       <c r="C13" s="52"/>
@@ -14111,7 +14118,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="116.25" customHeight="1">
       <c r="A14" s="52"/>
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
@@ -14123,7 +14130,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="116.25" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>130</v>
       </c>
@@ -14198,16 +14205,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -14230,16 +14237,16 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="37" t="s">
         <v>146</v>
       </c>
       <c r="E4" s="8"/>
@@ -14270,16 +14277,16 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="37" t="s">
         <v>154</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -14322,16 +14329,16 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="37" t="s">
         <v>168</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -14354,16 +14361,16 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="8" t="s">
         <v>176</v>
       </c>
@@ -15473,16 +15480,16 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>195</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -15505,16 +15512,16 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>203</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -15537,16 +15544,16 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>211</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -15605,16 +15612,16 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="111.75">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="38" t="s">
         <v>225</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -15637,16 +15644,16 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="38" t="s">
         <v>233</v>
       </c>
       <c r="E13" s="8" t="s">
@@ -15689,16 +15696,16 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="38" t="s">
         <v>247</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -15721,16 +15728,16 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="38" t="s">
         <v>255</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -15753,16 +15760,16 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="38" t="s">
         <v>262</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -15817,16 +15824,16 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="38" t="s">
         <v>278</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -15948,17 +15955,18 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="4" width="50.140625" customWidth="1"/>
+    <col min="6" max="6" width="24" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="12.75">
       <c r="A1" s="4" t="s">
         <v>76</v>
       </c>
@@ -15974,7 +15982,7 @@
       <c r="E1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -15994,27 +16002,27 @@
       <c r="E2" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="140.25" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>304</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>305</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>307</v>
       </c>
     </row>
@@ -16026,7 +16034,7 @@
       <c r="E4" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>309</v>
       </c>
     </row>
@@ -16046,11 +16054,11 @@
       <c r="E5" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="356.25">
       <c r="A6" s="8" t="s">
         <v>316</v>
       </c>
@@ -16066,11 +16074,11 @@
       <c r="E6" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="294.75">
       <c r="A7" s="8" t="s">
         <v>322</v>
       </c>
@@ -16086,11 +16094,11 @@
       <c r="E7" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="409.6">
       <c r="A8" s="8" t="s">
         <v>328</v>
       </c>
@@ -16106,11 +16114,11 @@
       <c r="E8" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="409.6">
       <c r="A9" s="8" t="s">
         <v>334</v>
       </c>
@@ -16126,11 +16134,11 @@
       <c r="E9" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="8" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="274.5">
       <c r="A10" s="8" t="s">
         <v>339</v>
       </c>
@@ -16146,11 +16154,11 @@
       <c r="E10" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="325.5">
       <c r="A11" s="8" t="s">
         <v>345</v>
       </c>
@@ -16166,11 +16174,11 @@
       <c r="E11" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="284.25">
       <c r="A12" s="8" t="s">
         <v>351</v>
       </c>
@@ -16186,7 +16194,7 @@
       <c r="E12" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>356</v>
       </c>
     </row>
@@ -16265,16 +16273,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="172.5">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="38" t="s">
         <v>366</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -16297,16 +16305,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="111.75">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="38" t="s">
         <v>374</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -16349,16 +16357,16 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="71.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="37" t="s">
         <v>385</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>386</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>387</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>388</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -16381,16 +16389,16 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="132">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="37" t="s">
         <v>393</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="37" t="s">
         <v>394</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="37" t="s">
         <v>395</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="38" t="s">
         <v>396</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -16413,16 +16421,16 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="172.5">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="37" t="s">
         <v>402</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="37" t="s">
         <v>403</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="38" t="s">
         <v>404</v>
       </c>
       <c r="E12" s="8" t="s">
@@ -16586,16 +16594,16 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>432</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>433</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="40" t="s">
         <v>434</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="41" t="s">
         <v>435</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -16618,16 +16626,16 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>440</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="40" t="s">
         <v>441</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="40" t="s">
         <v>442</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>443</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -16650,16 +16658,16 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="40" t="s">
         <v>448</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>449</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="40" t="s">
         <v>450</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="40" t="s">
         <v>451</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -17782,13 +17790,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>475</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>475</v>
       </c>
       <c r="D2" s="53" t="s">

</xml_diff>